<commit_message>
added measurements for query result bookmarking incremental xform
</commit_message>
<xml_diff>
--- a/tests/org.eclipse.incquery.examples.cps.performance.tests/results/XForm_CS_PS_Performance.xlsx
+++ b/tests/org.eclipse.incquery.examples.cps.performance.tests/results/XForm_CS_PS_Performance.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\work\demonstrator\ide\git\incquery-examples-cps\tests\org.eclipse.incquery.examples.cps.performance.tests\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\development\projects\demonstrator\ide\git\incquery-examples-cps.git\tests\org.eclipse.incquery.examples.cps.performance.tests\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="25">
   <si>
     <t>ClientServerScenario</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>AfterLastTrafo (KB)</t>
+  </si>
+  <si>
+    <t>QueryResultTraceability</t>
   </si>
 </sst>
 </file>
@@ -609,48 +612,48 @@
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="1. jelölőszín" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="2. jelölőszín" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="20% - 1. jelölőszín" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - 2. jelölőszín" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - 3. jelölőszín" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - 4. jelölőszín" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - 5. jelölőszín" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - 6. jelölőszín" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="3. jelölőszín" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="4. jelölőszín" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="40% - 1. jelölőszín" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - 2. jelölőszín" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - 3. jelölőszín" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - 4. jelölőszín" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - 5. jelölőszín" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - 6. jelölőszín" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="5. jelölőszín" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="6. jelölőszín" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="60% - 1. jelölőszín" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - 2. jelölőszín" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - 3. jelölőszín" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - 4. jelölőszín" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - 5. jelölőszín" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - 6. jelölőszín" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Bevitel" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Cím" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Címsor 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Címsor 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Címsor 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Címsor 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Ellenőrzőcella" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Figyelmeztetés" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Hivatkozott cella" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Jegyzet" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Jó" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Kimenet" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Magyarázó szöveg" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Normál" xfId="0" builtinId="0"/>
-    <cellStyle name="Összesen" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Rossz" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Semleges" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Számítás" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -668,7 +671,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="hu-HU"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1239,6 +1242,118 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Time!$C$45</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>QueryResultTraceability</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Time!$B$45:$B$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1024</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Time!$F$45:$F$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>691</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>914</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1322</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2698</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2903</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>17017</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>19364</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>55916</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>187333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -1247,11 +1362,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="278615648"/>
-        <c:axId val="278611728"/>
+        <c:axId val="-1975487968"/>
+        <c:axId val="-1975479264"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="278615648"/>
+        <c:axId val="-1975487968"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -1365,12 +1480,12 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="278611728"/>
+        <c:crossAx val="-1975479264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="278611728"/>
+        <c:axId val="-1975479264"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -1484,7 +1599,7 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="278615648"/>
+        <c:crossAx val="-1975487968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1568,7 +1683,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="hu-HU"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1654,7 +1769,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Time!$C$45</c:f>
+              <c:f>Time!$C$54</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1689,7 +1804,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Time!$B$45:$B$56</c:f>
+              <c:f>Time!$B$54:$B$65</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -1734,7 +1849,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Time!$F$45:$F$56</c:f>
+              <c:f>Time!$F$54:$F$65</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -1784,7 +1899,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Time!$C$57</c:f>
+              <c:f>Time!$C$66</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1819,7 +1934,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Time!$B$57:$B$63</c:f>
+              <c:f>Time!$B$66:$B$72</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1849,7 +1964,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Time!$F$57:$F$63</c:f>
+              <c:f>Time!$F$66:$F$72</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1884,7 +1999,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Time!$C$69</c:f>
+              <c:f>Time!$C$78</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1919,7 +2034,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Time!$B$69:$B$79</c:f>
+              <c:f>Time!$B$78:$B$88</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1961,7 +2076,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Time!$F$69:$F$79</c:f>
+              <c:f>Time!$F$78:$F$88</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2008,7 +2123,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Time!$C$64</c:f>
+              <c:f>Time!$C$73</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2043,7 +2158,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Time!$B$64:$B$68</c:f>
+              <c:f>Time!$B$73:$B$77</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2067,7 +2182,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Time!$F$64:$F$68</c:f>
+              <c:f>Time!$F$73:$F$77</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2085,6 +2200,118 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>39978</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Time!$C$89</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>QueryResultTraceability</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Time!$B$89:$B$97</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1024</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Time!$F$89:$F$97</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>638</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>967</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>894</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1178</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3509</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3560</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6063</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18451</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>32176</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2099,11 +2326,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="278612120"/>
-        <c:axId val="278612512"/>
+        <c:axId val="-1975475456"/>
+        <c:axId val="-1975490144"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="278612120"/>
+        <c:axId val="-1975475456"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -2217,12 +2444,12 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="278612512"/>
+        <c:crossAx val="-1975490144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="278612512"/>
+        <c:axId val="-1975490144"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -2336,7 +2563,7 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="278612120"/>
+        <c:crossAx val="-1975475456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2420,7 +2647,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="hu-HU"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2997,6 +3224,118 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Time!$C$45</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>QueryResultTraceability</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Time!$B$45:$B$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1024</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Time!$G$45:$G$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>202</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>104</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -3005,11 +3344,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="241485744"/>
-        <c:axId val="241486136"/>
+        <c:axId val="-1852048800"/>
+        <c:axId val="-1852053152"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="241485744"/>
+        <c:axId val="-1852048800"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -3123,12 +3462,12 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="241486136"/>
+        <c:crossAx val="-1852053152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="241486136"/>
+        <c:axId val="-1852053152"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -3242,7 +3581,7 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="241485744"/>
+        <c:crossAx val="-1852048800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="4"/>
@@ -3327,7 +3666,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="hu-HU"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3413,7 +3752,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Time!$C$45</c:f>
+              <c:f>Time!$C$54</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3448,7 +3787,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Time!$B$45:$B$56</c:f>
+              <c:f>Time!$B$54:$B$65</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -3493,7 +3832,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Time!$G$45:$G$56</c:f>
+              <c:f>Time!$G$54:$G$65</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -3543,7 +3882,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Time!$C$57</c:f>
+              <c:f>Time!$C$66</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3578,7 +3917,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Time!$B$57:$B$63</c:f>
+              <c:f>Time!$B$66:$B$72</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -3608,7 +3947,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Time!$G$57:$G$63</c:f>
+              <c:f>Time!$G$66:$G$72</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -3643,7 +3982,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Time!$C$69</c:f>
+              <c:f>Time!$C$78</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3678,7 +4017,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Time!$B$69:$B$79</c:f>
+              <c:f>Time!$B$78:$B$88</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -3720,7 +4059,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Time!$G$69:$G$79</c:f>
+              <c:f>Time!$G$78:$G$88</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -3767,7 +4106,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Time!$C$64</c:f>
+              <c:f>Time!$C$73</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3802,7 +4141,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Time!$B$64:$B$68</c:f>
+              <c:f>Time!$B$73:$B$77</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -3826,7 +4165,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Time!$G$64:$G$68</c:f>
+              <c:f>Time!$G$73:$G$77</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -3844,6 +4183,118 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>44263</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Time!$C$89</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>QueryResultTraceability</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Time!$B$89:$B$97</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1024</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Time!$G$89:$G$97</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>172</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3858,11 +4309,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="280358552"/>
-        <c:axId val="280353456"/>
+        <c:axId val="-1852046624"/>
+        <c:axId val="-1852043904"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="280358552"/>
+        <c:axId val="-1852046624"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -3976,12 +4427,12 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="280353456"/>
+        <c:crossAx val="-1852043904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="280353456"/>
+        <c:axId val="-1852043904"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -4095,7 +4546,7 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="280358552"/>
+        <c:crossAx val="-1852046624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4179,7 +4630,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="hu-HU"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4607,11 +5058,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="280358160"/>
-        <c:axId val="280351496"/>
+        <c:axId val="-1852055328"/>
+        <c:axId val="-1852055872"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="280358160"/>
+        <c:axId val="-1852055328"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -4725,12 +5176,12 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="280351496"/>
+        <c:crossAx val="-1852055872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="280351496"/>
+        <c:axId val="-1852055872"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -4845,7 +5296,7 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="280358160"/>
+        <c:crossAx val="-1852055328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4929,7 +5380,7 @@
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="hu-HU"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -5500,6 +5951,118 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Memory!$C$45</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>QueryResultTraceability</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Memory!$B$45:$B$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1024</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Memory!$E$45:$E$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>11.2783203125</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19.96875</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32.681640625</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>56.9609375</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>103.9814453125</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>308.158203125</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>375.4658203125</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>863.021484375</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1650.6123046875</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -5508,11 +6071,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="280354240"/>
-        <c:axId val="280353848"/>
+        <c:axId val="-1852046080"/>
+        <c:axId val="-1852054240"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="280354240"/>
+        <c:axId val="-1852046080"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -5626,12 +6189,12 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="280353848"/>
+        <c:crossAx val="-1852054240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="280353848"/>
+        <c:axId val="-1852054240"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -5746,7 +6309,7 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="280354240"/>
+        <c:crossAx val="-1852046080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5830,7 +6393,7 @@
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="hu-HU"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -5916,7 +6479,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Memory!$C$45</c:f>
+              <c:f>Memory!$C$54</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5951,7 +6514,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Memory!$B$45:$B$56</c:f>
+              <c:f>Memory!$B$54:$B$65</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -5996,7 +6559,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Memory!$E$45:$E$56</c:f>
+              <c:f>Memory!$E$54:$E$65</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -6046,7 +6609,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Memory!$C$57</c:f>
+              <c:f>Memory!$C$66</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6081,7 +6644,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Memory!$B$57:$B$63</c:f>
+              <c:f>Memory!$B$66:$B$72</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -6111,7 +6674,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Memory!$E$57:$E$63</c:f>
+              <c:f>Memory!$E$66:$E$72</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -6146,7 +6709,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Memory!$C$69</c:f>
+              <c:f>Memory!$C$78</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6181,7 +6744,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Memory!$B$69:$B$79</c:f>
+              <c:f>Memory!$B$78:$B$88</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -6223,7 +6786,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Memory!$E$69:$E$79</c:f>
+              <c:f>Memory!$E$78:$E$88</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -6270,7 +6833,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Memory!$C$64</c:f>
+              <c:f>Memory!$C$73</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6305,7 +6868,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Memory!$B$64:$B$68</c:f>
+              <c:f>Memory!$B$73:$B$77</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -6329,7 +6892,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Memory!$E$64:$E$68</c:f>
+              <c:f>Memory!$E$73:$E$77</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -6347,6 +6910,118 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>34.3896484375</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Memory!$C$89</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>QueryResultTraceability</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Memory!$B$89:$B$97</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1024</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Memory!$E$89:$E$97</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>11.1865234375</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19.2880859375</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>28.5595703125</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>47.0234375</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>83.724609375</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>156.685546875</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>303.8046875</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>599.650390625</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1197.705078125</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6361,11 +7036,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="280354632"/>
-        <c:axId val="280355808"/>
+        <c:axId val="-1852052064"/>
+        <c:axId val="-1852048256"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="280354632"/>
+        <c:axId val="-1852052064"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -6479,12 +7154,12 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="280355808"/>
+        <c:crossAx val="-1852048256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="280355808"/>
+        <c:axId val="-1852048256"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -6598,7 +7273,7 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="280354632"/>
+        <c:crossAx val="-1852052064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10811,7 +11486,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-téma">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -11073,17 +11748,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H90"/>
+  <dimension ref="A1:H99"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView topLeftCell="I20" workbookViewId="0">
+      <selection activeCell="AB37" sqref="AB37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
@@ -12115,462 +12790,466 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="B45" s="1">
         <v>1</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="D45" s="1">
-        <v>13</v>
+        <v>393</v>
       </c>
       <c r="E45" s="1">
-        <v>21</v>
+        <v>78</v>
       </c>
       <c r="F45" s="1">
-        <v>124</v>
+        <v>691</v>
       </c>
       <c r="G45" s="1">
-        <v>93</v>
+        <v>60</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="B46" s="1">
         <v>8</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="D46" s="1">
+        <v>183</v>
+      </c>
+      <c r="E46" s="1">
+        <v>40</v>
+      </c>
+      <c r="F46" s="1">
+        <v>914</v>
+      </c>
+      <c r="G46" s="1">
         <v>34</v>
       </c>
-      <c r="E46" s="1">
-        <v>24</v>
-      </c>
-      <c r="F46" s="1">
-        <v>169</v>
-      </c>
-      <c r="G46" s="1">
-        <v>152</v>
-      </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
-        <v>18</v>
+      <c r="A47" t="s">
+        <v>0</v>
       </c>
       <c r="B47" s="1">
         <v>16</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="D47" s="1">
-        <v>818</v>
+        <v>105</v>
       </c>
       <c r="E47" s="1">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="F47" s="1">
-        <v>1129</v>
+        <v>1322</v>
       </c>
       <c r="G47" s="1">
-        <v>459</v>
+        <v>30</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
-        <v>18</v>
+      <c r="A48" t="s">
+        <v>0</v>
       </c>
       <c r="B48" s="1">
         <v>32</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="D48" s="1">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="E48" s="1">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="F48" s="1">
-        <v>387</v>
+        <v>2698</v>
       </c>
       <c r="G48" s="1">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="4" t="s">
-        <v>18</v>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>0</v>
       </c>
       <c r="B49" s="1">
         <v>64</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="D49" s="1">
-        <v>146</v>
+        <v>217</v>
       </c>
       <c r="E49" s="1">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="F49" s="1">
-        <v>701</v>
+        <v>2903</v>
       </c>
       <c r="G49" s="1">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>0</v>
       </c>
       <c r="B50" s="1">
         <v>128</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="D50" s="1">
-        <v>243</v>
+        <v>2205</v>
       </c>
       <c r="E50" s="1">
-        <v>29</v>
+        <v>491</v>
       </c>
       <c r="F50" s="1">
-        <v>1230</v>
+        <v>17017</v>
       </c>
       <c r="G50" s="1">
-        <v>1269</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
-        <v>18</v>
+        <v>68</v>
+      </c>
+      <c r="H50"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>0</v>
       </c>
       <c r="B51" s="1">
         <v>256</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="D51" s="1">
-        <v>596</v>
+        <v>1034</v>
       </c>
       <c r="E51" s="1">
-        <v>57</v>
+        <v>145</v>
       </c>
       <c r="F51" s="1">
-        <v>2268</v>
+        <v>19364</v>
       </c>
       <c r="G51" s="1">
-        <v>2423</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="4" t="s">
-        <v>18</v>
+        <v>61</v>
+      </c>
+      <c r="H51"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>0</v>
       </c>
       <c r="B52" s="1">
         <v>512</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="D52" s="1">
-        <v>2933</v>
+        <v>2434</v>
       </c>
       <c r="E52" s="1">
-        <v>403</v>
+        <v>242</v>
       </c>
       <c r="F52" s="1">
-        <v>6250</v>
+        <v>55916</v>
       </c>
       <c r="G52" s="1">
-        <v>4348</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="4" t="s">
-        <v>18</v>
+        <v>202</v>
+      </c>
+      <c r="H52"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>0</v>
       </c>
       <c r="B53" s="1">
         <v>1024</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="D53" s="1">
-        <v>5420</v>
+        <v>6826</v>
       </c>
       <c r="E53" s="1">
-        <v>324</v>
+        <v>495</v>
       </c>
       <c r="F53" s="1">
-        <v>7616</v>
+        <v>187333</v>
       </c>
       <c r="G53" s="1">
-        <v>9909</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+      <c r="H53"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>18</v>
       </c>
       <c r="B54" s="1">
-        <v>1280</v>
+        <v>1</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D54" s="1">
-        <v>10060</v>
+        <v>13</v>
       </c>
       <c r="E54" s="1">
-        <v>470</v>
+        <v>21</v>
       </c>
       <c r="F54" s="1">
-        <v>11177</v>
+        <v>124</v>
       </c>
       <c r="G54" s="1">
-        <v>10286</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>18</v>
       </c>
       <c r="B55" s="1">
-        <v>1536</v>
+        <v>8</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D55" s="1">
-        <v>11887</v>
+        <v>34</v>
       </c>
       <c r="E55" s="1">
-        <v>361</v>
+        <v>24</v>
       </c>
       <c r="F55" s="1">
-        <v>12126</v>
+        <v>169</v>
       </c>
       <c r="G55" s="1">
-        <v>13776</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B56" s="1">
-        <v>2048</v>
+        <v>16</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D56" s="1">
-        <v>11487</v>
+        <v>818</v>
       </c>
       <c r="E56" s="1">
-        <v>513</v>
+        <v>57</v>
       </c>
       <c r="F56" s="1">
-        <v>13213</v>
+        <v>1129</v>
       </c>
       <c r="G56" s="1">
-        <v>14713</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B57" s="1">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D57" s="1">
-        <v>16</v>
+        <v>148</v>
       </c>
       <c r="E57" s="1">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F57" s="1">
-        <v>93</v>
+        <v>387</v>
       </c>
       <c r="G57" s="1">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B58" s="1">
-        <v>8</v>
+        <v>64</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D58" s="1">
-        <v>50</v>
+        <v>146</v>
       </c>
       <c r="E58" s="1">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="F58" s="1">
-        <v>188</v>
+        <v>701</v>
       </c>
       <c r="G58" s="1">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B59" s="1">
-        <v>16</v>
+        <v>128</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D59" s="1">
-        <v>685</v>
+        <v>243</v>
       </c>
       <c r="E59" s="1">
-        <v>88</v>
+        <v>29</v>
       </c>
       <c r="F59" s="1">
-        <v>1152</v>
+        <v>1230</v>
       </c>
       <c r="G59" s="1">
-        <v>667</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1269</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B60" s="1">
-        <v>32</v>
+        <v>256</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D60" s="1">
-        <v>204</v>
+        <v>596</v>
       </c>
       <c r="E60" s="1">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="F60" s="1">
-        <v>822</v>
+        <v>2268</v>
       </c>
       <c r="G60" s="1">
-        <v>1053</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2423</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B61" s="1">
-        <v>64</v>
+        <v>512</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D61" s="1">
-        <v>167</v>
+        <v>2933</v>
       </c>
       <c r="E61" s="1">
-        <v>35</v>
+        <v>403</v>
       </c>
       <c r="F61" s="1">
-        <v>4091</v>
+        <v>6250</v>
       </c>
       <c r="G61" s="1">
-        <v>3667</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4348</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B62" s="1">
-        <v>128</v>
+        <v>1024</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D62" s="1">
-        <v>271</v>
+        <v>5420</v>
       </c>
       <c r="E62" s="1">
-        <v>27</v>
+        <v>324</v>
       </c>
       <c r="F62" s="1">
-        <v>17054</v>
+        <v>7616</v>
       </c>
       <c r="G62" s="1">
-        <v>14678</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="4" t="s">
+        <v>9909</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>18</v>
       </c>
       <c r="B63" s="1">
-        <v>256</v>
+        <v>1280</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D63" s="1">
-        <v>473</v>
+        <v>10060</v>
       </c>
       <c r="E63" s="1">
-        <v>62</v>
+        <v>470</v>
       </c>
       <c r="F63" s="1">
-        <v>77935</v>
+        <v>11177</v>
       </c>
       <c r="G63" s="1">
-        <v>71400</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10286</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>18</v>
       </c>
       <c r="B64" s="1">
-        <v>1</v>
+        <v>1536</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D64" s="1">
-        <v>297</v>
+        <v>11887</v>
       </c>
       <c r="E64" s="1">
-        <v>65</v>
+        <v>361</v>
       </c>
       <c r="F64" s="1">
-        <v>141</v>
+        <v>12126</v>
       </c>
       <c r="G64" s="1">
-        <v>131</v>
+        <v>13776</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
@@ -12578,142 +13257,137 @@
         <v>18</v>
       </c>
       <c r="B65" s="1">
+        <v>2048</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D65" s="1">
+        <v>11487</v>
+      </c>
+      <c r="E65" s="1">
+        <v>513</v>
+      </c>
+      <c r="F65" s="1">
+        <v>13213</v>
+      </c>
+      <c r="G65" s="1">
+        <v>14713</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>18</v>
+      </c>
+      <c r="B66" s="1">
+        <v>1</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D66" s="1">
+        <v>16</v>
+      </c>
+      <c r="E66" s="1">
+        <v>20</v>
+      </c>
+      <c r="F66" s="1">
+        <v>93</v>
+      </c>
+      <c r="G66" s="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>18</v>
+      </c>
+      <c r="B67" s="1">
         <v>8</v>
       </c>
-      <c r="C65" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D65" s="1">
-        <v>127</v>
-      </c>
-      <c r="E65" s="1">
-        <v>34</v>
-      </c>
-      <c r="F65" s="1">
-        <v>727</v>
-      </c>
-      <c r="G65" s="1">
-        <v>675</v>
-      </c>
-      <c r="H65"/>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B66" s="1">
-        <v>16</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D66" s="1">
-        <v>672</v>
-      </c>
-      <c r="E66" s="1">
-        <v>86</v>
-      </c>
-      <c r="F66" s="1">
-        <v>3615</v>
-      </c>
-      <c r="G66" s="1">
-        <v>3009</v>
-      </c>
-      <c r="H66"/>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B67" s="1">
-        <v>32</v>
-      </c>
       <c r="C67" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D67" s="1">
-        <v>184</v>
+        <v>50</v>
       </c>
       <c r="E67" s="1">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F67" s="1">
-        <v>7654</v>
+        <v>188</v>
       </c>
       <c r="G67" s="1">
-        <v>7306</v>
-      </c>
-      <c r="H67"/>
+        <v>218</v>
+      </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B68" s="1">
+        <v>16</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D68" s="1">
+        <v>685</v>
+      </c>
+      <c r="E68" s="1">
+        <v>88</v>
+      </c>
+      <c r="F68" s="1">
+        <v>1152</v>
+      </c>
+      <c r="G68" s="1">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B69" s="1">
+        <v>32</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D69" s="1">
+        <v>204</v>
+      </c>
+      <c r="E69" s="1">
+        <v>27</v>
+      </c>
+      <c r="F69" s="1">
+        <v>822</v>
+      </c>
+      <c r="G69" s="1">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B70" s="1">
         <v>64</v>
       </c>
-      <c r="C68" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D68" s="1">
-        <v>142</v>
-      </c>
-      <c r="E68" s="1">
-        <v>23</v>
-      </c>
-      <c r="F68" s="1">
-        <v>39978</v>
-      </c>
-      <c r="G68" s="1">
-        <v>44263</v>
-      </c>
-      <c r="H68"/>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>18</v>
-      </c>
-      <c r="B69" s="1">
-        <v>1</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D69" s="1">
-        <v>8</v>
-      </c>
-      <c r="E69" s="1">
-        <v>12</v>
-      </c>
-      <c r="F69" s="1">
-        <v>419</v>
-      </c>
-      <c r="G69" s="1">
-        <v>31</v>
-      </c>
-      <c r="H69"/>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>18</v>
-      </c>
-      <c r="B70" s="1">
-        <v>8</v>
-      </c>
       <c r="C70" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D70" s="1">
-        <v>24</v>
+        <v>167</v>
       </c>
       <c r="E70" s="1">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="F70" s="1">
-        <v>553</v>
+        <v>4091</v>
       </c>
       <c r="G70" s="1">
-        <v>15</v>
+        <v>3667</v>
       </c>
       <c r="H70"/>
     </row>
@@ -12722,22 +13396,22 @@
         <v>18</v>
       </c>
       <c r="B71" s="1">
-        <v>16</v>
+        <v>128</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D71" s="1">
-        <v>55</v>
+        <v>271</v>
       </c>
       <c r="E71" s="1">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="F71" s="1">
-        <v>2028</v>
+        <v>17054</v>
       </c>
       <c r="G71" s="1">
-        <v>16</v>
+        <v>14678</v>
       </c>
       <c r="H71"/>
     </row>
@@ -12746,70 +13420,70 @@
         <v>18</v>
       </c>
       <c r="B72" s="1">
-        <v>32</v>
+        <v>256</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D72" s="1">
-        <v>48</v>
+        <v>473</v>
       </c>
       <c r="E72" s="1">
-        <v>7</v>
+        <v>62</v>
       </c>
       <c r="F72" s="1">
-        <v>1552</v>
+        <v>77935</v>
       </c>
       <c r="G72" s="1">
-        <v>2</v>
+        <v>71400</v>
       </c>
       <c r="H72"/>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" s="4" t="s">
+      <c r="A73" t="s">
         <v>18</v>
       </c>
       <c r="B73" s="1">
-        <v>64</v>
+        <v>1</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D73" s="1">
-        <v>90</v>
+        <v>297</v>
       </c>
       <c r="E73" s="1">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="F73" s="1">
-        <v>2753</v>
+        <v>141</v>
       </c>
       <c r="G73" s="1">
-        <v>4</v>
+        <v>131</v>
       </c>
       <c r="H73"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74" s="4" t="s">
+      <c r="A74" t="s">
         <v>18</v>
       </c>
       <c r="B74" s="1">
-        <v>128</v>
+        <v>8</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D74" s="1">
-        <v>264</v>
+        <v>127</v>
       </c>
       <c r="E74" s="1">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="F74" s="1">
-        <v>7032</v>
+        <v>727</v>
       </c>
       <c r="G74" s="1">
-        <v>6</v>
+        <v>675</v>
       </c>
       <c r="H74"/>
     </row>
@@ -12818,22 +13492,22 @@
         <v>18</v>
       </c>
       <c r="B75" s="1">
-        <v>256</v>
+        <v>16</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D75" s="1">
-        <v>405</v>
+        <v>672</v>
       </c>
       <c r="E75" s="1">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="F75" s="1">
-        <v>10925</v>
+        <v>3615</v>
       </c>
       <c r="G75" s="1">
-        <v>7</v>
+        <v>3009</v>
       </c>
       <c r="H75"/>
     </row>
@@ -12842,22 +13516,22 @@
         <v>18</v>
       </c>
       <c r="B76" s="1">
-        <v>512</v>
+        <v>32</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D76" s="1">
-        <v>2005</v>
+        <v>184</v>
       </c>
       <c r="E76" s="1">
-        <v>121</v>
+        <v>28</v>
       </c>
       <c r="F76" s="1">
-        <v>36657</v>
+        <v>7654</v>
       </c>
       <c r="G76" s="1">
-        <v>31</v>
+        <v>7306</v>
       </c>
       <c r="H76"/>
     </row>
@@ -12866,22 +13540,22 @@
         <v>18</v>
       </c>
       <c r="B77" s="1">
-        <v>1024</v>
+        <v>64</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D77" s="1">
-        <v>4689</v>
+        <v>142</v>
       </c>
       <c r="E77" s="1">
-        <v>310</v>
+        <v>23</v>
       </c>
       <c r="F77" s="1">
-        <v>109136</v>
+        <v>39978</v>
       </c>
       <c r="G77" s="1">
-        <v>13</v>
+        <v>44263</v>
       </c>
       <c r="H77"/>
     </row>
@@ -12890,22 +13564,22 @@
         <v>18</v>
       </c>
       <c r="B78" s="1">
-        <v>1280</v>
+        <v>1</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D78" s="1">
-        <v>6689</v>
+        <v>8</v>
       </c>
       <c r="E78" s="1">
-        <v>296</v>
+        <v>12</v>
       </c>
       <c r="F78" s="1">
-        <v>55550</v>
+        <v>419</v>
       </c>
       <c r="G78" s="1">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="H78"/>
     </row>
@@ -12914,217 +13588,220 @@
         <v>18</v>
       </c>
       <c r="B79" s="1">
-        <v>1536</v>
+        <v>8</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D79" s="1">
-        <v>8710</v>
+        <v>24</v>
       </c>
       <c r="E79" s="1">
-        <v>347</v>
+        <v>17</v>
       </c>
       <c r="F79" s="1">
-        <v>73343</v>
+        <v>553</v>
       </c>
       <c r="G79" s="1">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="H79"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>0</v>
+      <c r="A80" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="B80" s="1">
-        <v>1536</v>
+        <v>16</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D80" s="1">
-        <v>7869</v>
+        <v>55</v>
       </c>
       <c r="E80" s="1">
-        <v>623</v>
+        <v>5</v>
       </c>
       <c r="F80" s="1">
-        <v>29197</v>
+        <v>2028</v>
       </c>
       <c r="G80" s="1">
-        <v>29685</v>
+        <v>16</v>
       </c>
       <c r="H80"/>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>0</v>
+      <c r="A81" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="B81" s="1">
-        <v>2048</v>
+        <v>32</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D81" s="1">
-        <v>12698</v>
+        <v>48</v>
       </c>
       <c r="E81" s="1">
-        <v>460</v>
+        <v>7</v>
       </c>
       <c r="F81" s="1">
-        <v>31344</v>
+        <v>1552</v>
       </c>
       <c r="G81" s="1">
-        <v>32896</v>
+        <v>2</v>
       </c>
       <c r="H81"/>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>0</v>
+      <c r="A82" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="B82" s="1">
-        <v>2304</v>
+        <v>64</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D82" s="1">
-        <v>21623</v>
+        <v>90</v>
       </c>
       <c r="E82" s="1">
-        <v>506</v>
+        <v>12</v>
       </c>
       <c r="F82" s="1">
-        <v>35943</v>
+        <v>2753</v>
       </c>
       <c r="G82" s="1">
-        <v>38105</v>
+        <v>4</v>
       </c>
       <c r="H82"/>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>0</v>
+      <c r="A83" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="B83" s="1">
-        <v>2560</v>
+        <v>128</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D83" s="1">
-        <v>16499</v>
+        <v>264</v>
       </c>
       <c r="E83" s="1">
-        <v>549</v>
+        <v>23</v>
       </c>
       <c r="F83" s="1">
-        <v>44455</v>
+        <v>7032</v>
       </c>
       <c r="G83" s="1">
-        <v>46933</v>
+        <v>6</v>
       </c>
       <c r="H83"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>0</v>
+      <c r="A84" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="B84" s="1">
-        <v>3072</v>
+        <v>256</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D84" s="1">
-        <v>36332</v>
+        <v>405</v>
       </c>
       <c r="E84" s="1">
-        <v>629</v>
+        <v>62</v>
       </c>
       <c r="F84" s="1">
-        <v>38730</v>
+        <v>10925</v>
       </c>
       <c r="G84" s="1">
-        <v>41708</v>
+        <v>7</v>
       </c>
       <c r="H84"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>0</v>
+      <c r="A85" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="B85" s="1">
-        <v>3584</v>
+        <v>512</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D85" s="1">
-        <v>64133</v>
+        <v>2005</v>
       </c>
       <c r="E85" s="1">
-        <v>786</v>
+        <v>121</v>
       </c>
       <c r="F85" s="1">
-        <v>70202</v>
+        <v>36657</v>
       </c>
       <c r="G85" s="1">
-        <v>73538</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="H85"/>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>0</v>
+      <c r="A86" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="B86" s="1">
-        <v>4096</v>
+        <v>1024</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D86" s="1">
-        <v>62891</v>
+        <v>4689</v>
       </c>
       <c r="E86" s="1">
-        <v>936</v>
+        <v>310</v>
       </c>
       <c r="F86" s="1">
-        <v>70971</v>
+        <v>109136</v>
       </c>
       <c r="G86" s="1">
-        <v>86913</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="H86"/>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="B87" s="1">
-        <v>4608</v>
+        <v>1280</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D87" s="1">
-        <v>70252</v>
+        <v>6689</v>
       </c>
       <c r="E87" s="1">
-        <v>1021</v>
+        <v>296</v>
       </c>
       <c r="F87" s="1">
-        <v>98525</v>
+        <v>55550</v>
       </c>
       <c r="G87" s="1">
-        <v>102076</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="H87"/>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="B88" s="1">
         <v>1536</v>
@@ -13133,63 +13810,240 @@
         <v>4</v>
       </c>
       <c r="D88" s="1">
-        <v>5877</v>
+        <v>8710</v>
       </c>
       <c r="E88" s="1">
-        <v>317</v>
+        <v>347</v>
       </c>
       <c r="F88" s="1">
-        <v>121257</v>
+        <v>73343</v>
       </c>
       <c r="G88" s="1">
-        <v>61</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="H88"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="B89" s="1">
-        <v>2048</v>
+        <v>1</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="D89" s="1">
-        <v>13596</v>
+        <v>416</v>
       </c>
       <c r="E89" s="1">
-        <v>474</v>
+        <v>101</v>
       </c>
       <c r="F89" s="1">
-        <v>222379</v>
+        <v>638</v>
       </c>
       <c r="G89" s="1">
-        <v>47</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="H89"/>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="B90" s="1">
-        <v>2304</v>
+        <v>8</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="D90" s="1">
-        <v>21723</v>
+        <v>161</v>
       </c>
       <c r="E90" s="1">
-        <v>494</v>
+        <v>53</v>
       </c>
       <c r="F90" s="1">
-        <v>242683</v>
+        <v>967</v>
       </c>
       <c r="G90" s="1">
-        <v>54</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="H90"/>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>18</v>
+      </c>
+      <c r="B91" s="1">
+        <v>16</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D91" s="1">
+        <v>112</v>
+      </c>
+      <c r="E91" s="1">
+        <v>47</v>
+      </c>
+      <c r="F91" s="1">
+        <v>894</v>
+      </c>
+      <c r="G91" s="1">
+        <v>38</v>
+      </c>
+      <c r="H91"/>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>18</v>
+      </c>
+      <c r="B92" s="1">
+        <v>32</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D92" s="1">
+        <v>138</v>
+      </c>
+      <c r="E92" s="1">
+        <v>78</v>
+      </c>
+      <c r="F92" s="1">
+        <v>1178</v>
+      </c>
+      <c r="G92" s="1">
+        <v>35</v>
+      </c>
+      <c r="H92"/>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>18</v>
+      </c>
+      <c r="B93" s="1">
+        <v>64</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D93" s="1">
+        <v>259</v>
+      </c>
+      <c r="E93" s="1">
+        <v>84</v>
+      </c>
+      <c r="F93" s="1">
+        <v>3509</v>
+      </c>
+      <c r="G93" s="1">
+        <v>9</v>
+      </c>
+      <c r="H93"/>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>18</v>
+      </c>
+      <c r="B94" s="1">
+        <v>128</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D94" s="1">
+        <v>437</v>
+      </c>
+      <c r="E94" s="1">
+        <v>126</v>
+      </c>
+      <c r="F94" s="1">
+        <v>3560</v>
+      </c>
+      <c r="G94" s="1">
+        <v>24</v>
+      </c>
+      <c r="H94"/>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>18</v>
+      </c>
+      <c r="B95" s="1">
+        <v>256</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D95" s="1">
+        <v>812</v>
+      </c>
+      <c r="E95" s="1">
+        <v>163</v>
+      </c>
+      <c r="F95" s="1">
+        <v>6063</v>
+      </c>
+      <c r="G95" s="1">
+        <v>20</v>
+      </c>
+      <c r="H95"/>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>18</v>
+      </c>
+      <c r="B96" s="1">
+        <v>512</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D96" s="1">
+        <v>2016</v>
+      </c>
+      <c r="E96" s="1">
+        <v>204</v>
+      </c>
+      <c r="F96" s="1">
+        <v>18451</v>
+      </c>
+      <c r="G96" s="1">
+        <v>43</v>
+      </c>
+      <c r="H96"/>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>18</v>
+      </c>
+      <c r="B97" s="1">
+        <v>1024</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D97" s="1">
+        <v>6791</v>
+      </c>
+      <c r="E97" s="1">
+        <v>399</v>
+      </c>
+      <c r="F97" s="1">
+        <v>32176</v>
+      </c>
+      <c r="G97" s="1">
+        <v>172</v>
+      </c>
+      <c r="H97"/>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A98"/>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A99"/>
     </row>
   </sheetData>
   <sortState ref="A2:G78">
@@ -16040,10 +16894,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G85"/>
+  <dimension ref="A1:G97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
+      <selection activeCell="C100" sqref="C100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16949,182 +17803,182 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="B45" s="1">
         <v>1</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="D45" s="1">
-        <v>30429</v>
+        <v>71906</v>
       </c>
       <c r="E45" s="1">
-        <v>108.978515625</v>
+        <v>11.2783203125</v>
       </c>
       <c r="F45" s="1">
-        <v>33246</v>
+        <v>11646</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="B46" s="1">
         <v>8</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="D46" s="1">
-        <v>33560</v>
+        <v>13553</v>
       </c>
       <c r="E46" s="1">
-        <v>39.1572265625</v>
+        <v>19.96875</v>
       </c>
       <c r="F46" s="1">
-        <v>41177</v>
+        <v>20741</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="B47" s="1">
         <v>16</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="D47" s="1">
-        <v>148702</v>
+        <v>26016</v>
       </c>
       <c r="E47" s="1">
-        <v>32.658203125</v>
+        <v>32.681640625</v>
       </c>
       <c r="F47" s="1">
-        <v>35259</v>
+        <v>33992</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="B48" s="1">
         <v>32</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="D48" s="1">
-        <v>33656</v>
+        <v>65134</v>
       </c>
       <c r="E48" s="1">
-        <v>48.17578125</v>
+        <v>56.9609375</v>
       </c>
       <c r="F48" s="1">
-        <v>52943</v>
+        <v>59280</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="B49" s="1">
         <v>64</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="D49" s="1">
-        <v>50412</v>
+        <v>79144</v>
       </c>
       <c r="E49" s="1">
-        <v>79.892578125</v>
+        <v>103.9814453125</v>
       </c>
       <c r="F49" s="1">
-        <v>141265</v>
+        <v>108226</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="B50" s="1">
         <v>128</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="D50" s="1">
-        <v>84589</v>
+        <v>90273</v>
       </c>
       <c r="E50" s="1">
-        <v>143.466796875</v>
+        <v>308.158203125</v>
       </c>
       <c r="F50" s="1">
-        <v>160680</v>
+        <v>219584</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="B51" s="1">
         <v>256</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="D51" s="1">
-        <v>151603</v>
+        <v>297735</v>
       </c>
       <c r="E51" s="1">
-        <v>270.912109375</v>
+        <v>375.4658203125</v>
       </c>
       <c r="F51" s="1">
-        <v>304740</v>
+        <v>431109</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="B52" s="1">
         <v>512</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="D52" s="1">
-        <v>203529</v>
+        <v>546005</v>
       </c>
       <c r="E52" s="1">
-        <v>541.1083984375</v>
+        <v>863.021484375</v>
       </c>
       <c r="F52" s="1">
-        <v>608139</v>
+        <v>897255</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="B53" s="1">
         <v>1024</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="D53" s="1">
-        <v>593116</v>
+        <v>1214117</v>
       </c>
       <c r="E53" s="1">
-        <v>1071.5068359375</v>
+        <v>1650.6123046875</v>
       </c>
       <c r="F53" s="1">
-        <v>1204256</v>
+        <v>1717042</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -17132,19 +17986,19 @@
         <v>18</v>
       </c>
       <c r="B54" s="1">
-        <v>1280</v>
+        <v>1</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D54" s="1">
-        <v>331918</v>
+        <v>30429</v>
       </c>
       <c r="E54" s="1">
-        <v>1347.2314453125</v>
+        <v>108.978515625</v>
       </c>
       <c r="F54" s="1">
-        <v>1513187</v>
+        <v>33246</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -17152,19 +18006,19 @@
         <v>18</v>
       </c>
       <c r="B55" s="1">
-        <v>1536</v>
+        <v>8</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D55" s="1">
-        <v>1201996</v>
+        <v>33560</v>
       </c>
       <c r="E55" s="1">
-        <v>1607.919921875</v>
+        <v>39.1572265625</v>
       </c>
       <c r="F55" s="1">
-        <v>1807929</v>
+        <v>41177</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -17172,19 +18026,19 @@
         <v>18</v>
       </c>
       <c r="B56" s="1">
-        <v>2048</v>
+        <v>16</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D56" s="1">
-        <v>1460368</v>
+        <v>148702</v>
       </c>
       <c r="E56" s="1">
-        <v>2176.1015625</v>
+        <v>32.658203125</v>
       </c>
       <c r="F56" s="1">
-        <v>2441838</v>
+        <v>35259</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -17192,19 +18046,19 @@
         <v>18</v>
       </c>
       <c r="B57" s="1">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D57" s="1">
-        <v>23010</v>
+        <v>33656</v>
       </c>
       <c r="E57" s="1">
-        <v>22.7421875</v>
+        <v>48.17578125</v>
       </c>
       <c r="F57" s="1">
-        <v>23335</v>
+        <v>52943</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -17212,19 +18066,19 @@
         <v>18</v>
       </c>
       <c r="B58" s="1">
-        <v>8</v>
+        <v>64</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D58" s="1">
-        <v>25559</v>
+        <v>50412</v>
       </c>
       <c r="E58" s="1">
-        <v>24.912109375</v>
+        <v>79.892578125</v>
       </c>
       <c r="F58" s="1">
-        <v>25737</v>
+        <v>141265</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -17232,19 +18086,19 @@
         <v>18</v>
       </c>
       <c r="B59" s="1">
-        <v>16</v>
+        <v>128</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D59" s="1">
-        <v>207334</v>
+        <v>84589</v>
       </c>
       <c r="E59" s="1">
-        <v>20.544921875</v>
+        <v>143.466796875</v>
       </c>
       <c r="F59" s="1">
-        <v>21410</v>
+        <v>160680</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -17252,19 +18106,19 @@
         <v>18</v>
       </c>
       <c r="B60" s="1">
-        <v>32</v>
+        <v>256</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D60" s="1">
-        <v>34281</v>
+        <v>151603</v>
       </c>
       <c r="E60" s="1">
-        <v>25.4189453125</v>
+        <v>270.912109375</v>
       </c>
       <c r="F60" s="1">
-        <v>26807</v>
+        <v>304740</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -17272,19 +18126,19 @@
         <v>18</v>
       </c>
       <c r="B61" s="1">
-        <v>64</v>
+        <v>512</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D61" s="1">
-        <v>51744</v>
+        <v>203529</v>
       </c>
       <c r="E61" s="1">
-        <v>164.5615234375</v>
+        <v>541.1083984375</v>
       </c>
       <c r="F61" s="1">
-        <v>38259</v>
+        <v>608139</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -17292,19 +18146,19 @@
         <v>18</v>
       </c>
       <c r="B62" s="1">
-        <v>128</v>
+        <v>1024</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D62" s="1">
-        <v>87376</v>
+        <v>593116</v>
       </c>
       <c r="E62" s="1">
-        <v>55.583984375</v>
+        <v>1071.5068359375</v>
       </c>
       <c r="F62" s="1">
-        <v>59899</v>
+        <v>1204256</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -17312,19 +18166,19 @@
         <v>18</v>
       </c>
       <c r="B63" s="1">
-        <v>256</v>
+        <v>1280</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D63" s="1">
-        <v>157235</v>
+        <v>331918</v>
       </c>
       <c r="E63" s="1">
-        <v>114.1259765625</v>
+        <v>1347.2314453125</v>
       </c>
       <c r="F63" s="1">
-        <v>103303</v>
+        <v>1513187</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -17332,19 +18186,19 @@
         <v>18</v>
       </c>
       <c r="B64" s="1">
-        <v>1</v>
+        <v>1536</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D64" s="1">
-        <v>205355</v>
+        <v>1201996</v>
       </c>
       <c r="E64" s="1">
-        <v>15.8818359375</v>
+        <v>1607.919921875</v>
       </c>
       <c r="F64" s="1">
-        <v>16218</v>
+        <v>1807929</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -17352,19 +18206,19 @@
         <v>18</v>
       </c>
       <c r="B65" s="1">
-        <v>8</v>
+        <v>2048</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D65" s="1">
-        <v>18449</v>
+        <v>1460368</v>
       </c>
       <c r="E65" s="1">
-        <v>17.857421875</v>
+        <v>2176.1015625</v>
       </c>
       <c r="F65" s="1">
-        <v>18299</v>
+        <v>2441838</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -17372,19 +18226,19 @@
         <v>18</v>
       </c>
       <c r="B66" s="1">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D66" s="1">
-        <v>207347</v>
+        <v>23010</v>
       </c>
       <c r="E66" s="1">
-        <v>20.181640625</v>
+        <v>22.7421875</v>
       </c>
       <c r="F66" s="1">
-        <v>20638</v>
+        <v>23335</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -17392,19 +18246,19 @@
         <v>18</v>
       </c>
       <c r="B67" s="1">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D67" s="1">
-        <v>33487</v>
+        <v>25559</v>
       </c>
       <c r="E67" s="1">
-        <v>25.259765625</v>
+        <v>24.912109375</v>
       </c>
       <c r="F67" s="1">
-        <v>25867</v>
+        <v>25737</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -17412,19 +18266,19 @@
         <v>18</v>
       </c>
       <c r="B68" s="1">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D68" s="1">
-        <v>50733</v>
+        <v>207334</v>
       </c>
       <c r="E68" s="1">
-        <v>34.3896484375</v>
+        <v>20.544921875</v>
       </c>
       <c r="F68" s="1">
-        <v>35276</v>
+        <v>21410</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -17432,19 +18286,19 @@
         <v>18</v>
       </c>
       <c r="B69" s="1">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D69" s="1">
-        <v>38142</v>
+        <v>34281</v>
       </c>
       <c r="E69" s="1">
-        <v>43.9130859375</v>
+        <v>25.4189453125</v>
       </c>
       <c r="F69" s="1">
-        <v>44607</v>
+        <v>26807</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -17452,19 +18306,19 @@
         <v>18</v>
       </c>
       <c r="B70" s="1">
-        <v>8</v>
+        <v>64</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D70" s="1">
-        <v>40983</v>
+        <v>51744</v>
       </c>
       <c r="E70" s="1">
-        <v>60.052734375</v>
+        <v>164.5615234375</v>
       </c>
       <c r="F70" s="1">
-        <v>61650</v>
+        <v>38259</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -17472,19 +18326,19 @@
         <v>18</v>
       </c>
       <c r="B71" s="1">
-        <v>16</v>
+        <v>128</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D71" s="1">
-        <v>219003</v>
+        <v>87376</v>
       </c>
       <c r="E71" s="1">
-        <v>267.9677734375</v>
+        <v>55.583984375</v>
       </c>
       <c r="F71" s="1">
-        <v>327855</v>
+        <v>59899</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -17492,19 +18346,19 @@
         <v>18</v>
       </c>
       <c r="B72" s="1">
-        <v>32</v>
+        <v>256</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D72" s="1">
-        <v>234922</v>
+        <v>157235</v>
       </c>
       <c r="E72" s="1">
-        <v>304.619140625</v>
+        <v>114.1259765625</v>
       </c>
       <c r="F72" s="1">
-        <v>312137</v>
+        <v>103303</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -17512,19 +18366,19 @@
         <v>18</v>
       </c>
       <c r="B73" s="1">
-        <v>64</v>
+        <v>1</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D73" s="1">
-        <v>251670</v>
+        <v>205355</v>
       </c>
       <c r="E73" s="1">
-        <v>381.3505859375</v>
+        <v>15.8818359375</v>
       </c>
       <c r="F73" s="1">
-        <v>391003</v>
+        <v>16218</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -17532,19 +18386,19 @@
         <v>18</v>
       </c>
       <c r="B74" s="1">
-        <v>128</v>
+        <v>8</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D74" s="1">
-        <v>285258</v>
+        <v>18449</v>
       </c>
       <c r="E74" s="1">
-        <v>559.9638671875</v>
+        <v>17.857421875</v>
       </c>
       <c r="F74" s="1">
-        <v>546979</v>
+        <v>18299</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -17552,19 +18406,19 @@
         <v>18</v>
       </c>
       <c r="B75" s="1">
-        <v>256</v>
+        <v>16</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D75" s="1">
-        <v>352182</v>
+        <v>207347</v>
       </c>
       <c r="E75" s="1">
-        <v>842.126953125</v>
+        <v>20.181640625</v>
       </c>
       <c r="F75" s="1">
-        <v>898484</v>
+        <v>20638</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -17572,19 +18426,19 @@
         <v>18</v>
       </c>
       <c r="B76" s="1">
-        <v>512</v>
+        <v>32</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D76" s="1">
-        <v>922155</v>
+        <v>33487</v>
       </c>
       <c r="E76" s="1">
-        <v>2252.7060546875</v>
+        <v>25.259765625</v>
       </c>
       <c r="F76" s="1">
-        <v>2308339</v>
+        <v>25867</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -17592,19 +18446,19 @@
         <v>18</v>
       </c>
       <c r="B77" s="1">
-        <v>1024</v>
+        <v>64</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D77" s="1">
-        <v>1350176</v>
+        <v>50733</v>
       </c>
       <c r="E77" s="1">
-        <v>3960.66015625</v>
+        <v>34.3896484375</v>
       </c>
       <c r="F77" s="1">
-        <v>4058669</v>
+        <v>35276</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
@@ -17612,19 +18466,19 @@
         <v>18</v>
       </c>
       <c r="B78" s="1">
-        <v>1280</v>
+        <v>1</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D78" s="1">
-        <v>1772780</v>
+        <v>38142</v>
       </c>
       <c r="E78" s="1">
-        <v>4994.587890625</v>
+        <v>43.9130859375</v>
       </c>
       <c r="F78" s="1">
-        <v>5117864</v>
+        <v>44607</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -17632,62 +18486,380 @@
         <v>18</v>
       </c>
       <c r="B79" s="1">
-        <v>1536</v>
+        <v>8</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D79" s="1">
+        <v>40983</v>
+      </c>
+      <c r="E79" s="1">
+        <v>60.052734375</v>
+      </c>
+      <c r="F79" s="1">
+        <v>61650</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>18</v>
+      </c>
+      <c r="B80" s="1">
+        <v>16</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D80" s="1">
+        <v>219003</v>
+      </c>
+      <c r="E80" s="1">
+        <v>267.9677734375</v>
+      </c>
+      <c r="F80" s="1">
+        <v>327855</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>18</v>
+      </c>
+      <c r="B81" s="1">
+        <v>32</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D81" s="1">
+        <v>234922</v>
+      </c>
+      <c r="E81" s="1">
+        <v>304.619140625</v>
+      </c>
+      <c r="F81" s="1">
+        <v>312137</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>18</v>
+      </c>
+      <c r="B82" s="1">
+        <v>64</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D82" s="1">
+        <v>251670</v>
+      </c>
+      <c r="E82" s="1">
+        <v>381.3505859375</v>
+      </c>
+      <c r="F82" s="1">
+        <v>391003</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>18</v>
+      </c>
+      <c r="B83" s="1">
+        <v>128</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D83" s="1">
+        <v>285258</v>
+      </c>
+      <c r="E83" s="1">
+        <v>559.9638671875</v>
+      </c>
+      <c r="F83" s="1">
+        <v>546979</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>18</v>
+      </c>
+      <c r="B84" s="1">
+        <v>256</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D84" s="1">
+        <v>352182</v>
+      </c>
+      <c r="E84" s="1">
+        <v>842.126953125</v>
+      </c>
+      <c r="F84" s="1">
+        <v>898484</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>18</v>
+      </c>
+      <c r="B85" s="1">
+        <v>512</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D85" s="1">
+        <v>922155</v>
+      </c>
+      <c r="E85" s="1">
+        <v>2252.7060546875</v>
+      </c>
+      <c r="F85" s="1">
+        <v>2308339</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>18</v>
+      </c>
+      <c r="B86" s="1">
+        <v>1024</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D86" s="1">
+        <v>1350176</v>
+      </c>
+      <c r="E86" s="1">
+        <v>3960.66015625</v>
+      </c>
+      <c r="F86" s="1">
+        <v>4058669</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>18</v>
+      </c>
+      <c r="B87" s="1">
+        <v>1280</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D87" s="1">
+        <v>1772780</v>
+      </c>
+      <c r="E87" s="1">
+        <v>4994.587890625</v>
+      </c>
+      <c r="F87" s="1">
+        <v>5117864</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>18</v>
+      </c>
+      <c r="B88" s="1">
+        <v>1536</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D88" s="1">
         <v>2791972</v>
       </c>
-      <c r="E79" s="1">
+      <c r="E88" s="1">
         <v>5722.361328125</v>
       </c>
-      <c r="F79" s="1">
+      <c r="F88" s="1">
         <v>5863874</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B80"/>
-      <c r="C80"/>
-      <c r="D80"/>
-      <c r="E80"/>
-      <c r="F80"/>
-    </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B81"/>
-      <c r="C81"/>
-      <c r="D81"/>
-      <c r="E81"/>
-      <c r="F81"/>
-    </row>
-    <row r="82" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B82"/>
-      <c r="C82"/>
-      <c r="D82"/>
-      <c r="E82"/>
-      <c r="F82"/>
-    </row>
-    <row r="83" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B83"/>
-      <c r="C83"/>
-      <c r="D83"/>
-      <c r="E83"/>
-      <c r="F83"/>
-    </row>
-    <row r="84" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B84"/>
-      <c r="C84"/>
-      <c r="D84"/>
-      <c r="E84"/>
-      <c r="F84"/>
-    </row>
-    <row r="85" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B85"/>
-      <c r="C85"/>
-      <c r="D85"/>
-      <c r="E85"/>
-      <c r="F85"/>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>18</v>
+      </c>
+      <c r="B89" s="1">
+        <v>1</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D89" s="1">
+        <v>71899</v>
+      </c>
+      <c r="E89" s="1">
+        <v>11.1865234375</v>
+      </c>
+      <c r="F89" s="1">
+        <v>11549</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>18</v>
+      </c>
+      <c r="B90" s="1">
+        <v>8</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D90" s="1">
+        <v>13345</v>
+      </c>
+      <c r="E90" s="1">
+        <v>19.2880859375</v>
+      </c>
+      <c r="F90" s="1">
+        <v>20037</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>18</v>
+      </c>
+      <c r="B91" s="1">
+        <v>16</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D91" s="1">
+        <v>25083</v>
+      </c>
+      <c r="E91" s="1">
+        <v>28.5595703125</v>
+      </c>
+      <c r="F91" s="1">
+        <v>29740</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>18</v>
+      </c>
+      <c r="B92" s="1">
+        <v>32</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D92" s="1">
+        <v>60350</v>
+      </c>
+      <c r="E92" s="1">
+        <v>47.0234375</v>
+      </c>
+      <c r="F92" s="1">
+        <v>49071</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>18</v>
+      </c>
+      <c r="B93" s="1">
+        <v>64</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D93" s="1">
+        <v>67776</v>
+      </c>
+      <c r="E93" s="1">
+        <v>83.724609375</v>
+      </c>
+      <c r="F93" s="1">
+        <v>87499</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>18</v>
+      </c>
+      <c r="B94" s="1">
+        <v>128</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D94" s="1">
+        <v>124362</v>
+      </c>
+      <c r="E94" s="1">
+        <v>156.685546875</v>
+      </c>
+      <c r="F94" s="1">
+        <v>163900</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>18</v>
+      </c>
+      <c r="B95" s="1">
+        <v>256</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D95" s="1">
+        <v>236992</v>
+      </c>
+      <c r="E95" s="1">
+        <v>303.8046875</v>
+      </c>
+      <c r="F95" s="1">
+        <v>317923</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>18</v>
+      </c>
+      <c r="B96" s="1">
+        <v>512</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D96" s="1">
+        <v>463360</v>
+      </c>
+      <c r="E96" s="1">
+        <v>599.650390625</v>
+      </c>
+      <c r="F96" s="1">
+        <v>627606</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>18</v>
+      </c>
+      <c r="B97" s="1">
+        <v>1024</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D97" s="1">
+        <v>927239</v>
+      </c>
+      <c r="E97" s="1">
+        <v>1197.705078125</v>
+      </c>
+      <c r="F97" s="1">
+        <v>1256716</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A2:H75">

</xml_diff>

<commit_message>
measured incr.qrt up to 3072
</commit_message>
<xml_diff>
--- a/tests/org.eclipse.incquery.examples.cps.performance.tests/results/XForm_CS_PS_Performance.xlsx
+++ b/tests/org.eclipse.incquery.examples.cps.performance.tests/results/XForm_CS_PS_Performance.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\development\projects\demonstrator\ide\git\incquery-examples-cps.git\tests\org.eclipse.incquery.examples.cps.performance.tests\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\work\demonstrator\ide\git\incquery-examples-cps\tests\org.eclipse.incquery.examples.cps.performance.tests\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Time" sheetId="4" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="25">
   <si>
     <t>ClientServerScenario</t>
   </si>
@@ -612,48 +612,48 @@
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="1. jelölőszín" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="2. jelölőszín" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="20% - 1. jelölőszín" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - 2. jelölőszín" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - 3. jelölőszín" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - 4. jelölőszín" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - 5. jelölőszín" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - 6. jelölőszín" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="3. jelölőszín" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="4. jelölőszín" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="40% - 1. jelölőszín" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - 2. jelölőszín" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - 3. jelölőszín" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - 4. jelölőszín" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - 5. jelölőszín" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - 6. jelölőszín" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="5. jelölőszín" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="6. jelölőszín" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="60% - 1. jelölőszín" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - 2. jelölőszín" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - 3. jelölőszín" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - 4. jelölőszín" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - 5. jelölőszín" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - 6. jelölőszín" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Bevitel" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Cím" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Címsor 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Címsor 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Címsor 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Címsor 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Ellenőrzőcella" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Figyelmeztetés" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Hivatkozott cella" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Jegyzet" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Jó" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Kimenet" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Magyarázó szöveg" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Normál" xfId="0" builtinId="0"/>
+    <cellStyle name="Összesen" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Rossz" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Semleges" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Számítás" xfId="11" builtinId="22" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -671,7 +671,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="hu-HU"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1282,10 +1282,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Time!$B$45:$B$53</c:f>
+              <c:f>Time!$B$45:$B$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1312,42 +1312,78 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1280</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1536</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2304</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2560</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3072</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Time!$F$45:$F$53</c:f>
+              <c:f>Time!$F$45:$F$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>691</c:v>
+                  <c:v>1728</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>914</c:v>
+                  <c:v>2473</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1322</c:v>
+                  <c:v>2119</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2698</c:v>
+                  <c:v>3179</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2903</c:v>
+                  <c:v>4977</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17017</c:v>
+                  <c:v>6699</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>19364</c:v>
+                  <c:v>21218</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>55916</c:v>
+                  <c:v>41665</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>187333</c:v>
+                  <c:v>97030</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>162317</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>138240</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>337698</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>379205</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>351245</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>214484</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1362,11 +1398,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1975487968"/>
-        <c:axId val="-1975479264"/>
+        <c:axId val="332366192"/>
+        <c:axId val="332368152"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1975487968"/>
+        <c:axId val="332366192"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -1480,12 +1516,12 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1975479264"/>
+        <c:crossAx val="332368152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1975479264"/>
+        <c:axId val="332368152"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -1599,7 +1635,7 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1975487968"/>
+        <c:crossAx val="332366192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1683,7 +1719,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="hu-HU"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1769,7 +1805,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Time!$C$54</c:f>
+              <c:f>Time!$C$60</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1804,7 +1840,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Time!$B$54:$B$65</c:f>
+              <c:f>Time!$B$60:$B$71</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -1849,7 +1885,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Time!$F$54:$F$65</c:f>
+              <c:f>Time!$F$60:$F$71</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -1899,7 +1935,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Time!$C$66</c:f>
+              <c:f>Time!$C$72</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1934,7 +1970,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Time!$B$66:$B$72</c:f>
+              <c:f>Time!$B$72:$B$78</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1964,7 +2000,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Time!$F$66:$F$72</c:f>
+              <c:f>Time!$F$72:$F$78</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1999,7 +2035,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Time!$C$78</c:f>
+              <c:f>Time!$C$84</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2034,7 +2070,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Time!$B$78:$B$88</c:f>
+              <c:f>Time!$B$84:$B$94</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2076,7 +2112,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Time!$F$78:$F$88</c:f>
+              <c:f>Time!$F$84:$F$94</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2123,7 +2159,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Time!$C$73</c:f>
+              <c:f>Time!$C$79</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2158,7 +2194,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Time!$B$73:$B$77</c:f>
+              <c:f>Time!$B$79:$B$83</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2182,7 +2218,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Time!$F$73:$F$77</c:f>
+              <c:f>Time!$F$79:$F$83</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2211,7 +2247,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Time!$C$89</c:f>
+              <c:f>Time!$C$95</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2246,10 +2282,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Time!$B$89:$B$97</c:f>
+              <c:f>Time!$B$95:$B$109</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -2276,42 +2312,78 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1280</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1536</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2304</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2560</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3072</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Time!$F$89:$F$97</c:f>
+              <c:f>Time!$F$95:$F$109</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>638</c:v>
+                  <c:v>1669</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>967</c:v>
+                  <c:v>1867</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>894</c:v>
+                  <c:v>1905</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1178</c:v>
+                  <c:v>2020</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3509</c:v>
+                  <c:v>2927</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3560</c:v>
+                  <c:v>4119</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6063</c:v>
+                  <c:v>5879</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>18451</c:v>
+                  <c:v>13580</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>32176</c:v>
+                  <c:v>27465</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>31295</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43129</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>51263</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>72592</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>86368</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>86160</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2326,11 +2398,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1975475456"/>
-        <c:axId val="-1975490144"/>
+        <c:axId val="332371288"/>
+        <c:axId val="332371680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1975475456"/>
+        <c:axId val="332371288"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -2444,12 +2516,12 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1975490144"/>
+        <c:crossAx val="332371680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1975490144"/>
+        <c:axId val="332371680"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -2563,7 +2635,7 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1975475456"/>
+        <c:crossAx val="332371288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2647,7 +2719,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="hu-HU"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3264,10 +3336,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Time!$B$45:$B$53</c:f>
+              <c:f>Time!$B$45:$B$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -3294,42 +3366,78 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1280</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1536</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2304</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2560</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3072</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Time!$G$45:$G$53</c:f>
+              <c:f>Time!$G$45:$G$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>60</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>34</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>51</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>68</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>61</c:v>
-                </c:pt>
                 <c:pt idx="7">
-                  <c:v>202</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>104</c:v>
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>188</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>191</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>221</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>265</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3344,11 +3452,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1852048800"/>
-        <c:axId val="-1852053152"/>
+        <c:axId val="332368544"/>
+        <c:axId val="110520768"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1852048800"/>
+        <c:axId val="332368544"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -3462,12 +3570,12 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1852053152"/>
+        <c:crossAx val="110520768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1852053152"/>
+        <c:axId val="110520768"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -3581,7 +3689,7 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1852048800"/>
+        <c:crossAx val="332368544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="4"/>
@@ -3666,7 +3774,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="hu-HU"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3752,7 +3860,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Time!$C$54</c:f>
+              <c:f>Time!$C$60</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3787,7 +3895,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Time!$B$54:$B$65</c:f>
+              <c:f>Time!$B$60:$B$71</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -3832,7 +3940,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Time!$G$54:$G$65</c:f>
+              <c:f>Time!$G$60:$G$71</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -3882,7 +3990,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Time!$C$66</c:f>
+              <c:f>Time!$C$72</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3917,7 +4025,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Time!$B$66:$B$72</c:f>
+              <c:f>Time!$B$72:$B$78</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -3947,7 +4055,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Time!$G$66:$G$72</c:f>
+              <c:f>Time!$G$72:$G$78</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -3982,7 +4090,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Time!$C$78</c:f>
+              <c:f>Time!$C$84</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4017,7 +4125,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Time!$B$78:$B$88</c:f>
+              <c:f>Time!$B$84:$B$94</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -4059,7 +4167,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Time!$G$78:$G$88</c:f>
+              <c:f>Time!$G$84:$G$94</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -4106,7 +4214,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Time!$C$73</c:f>
+              <c:f>Time!$C$79</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4141,7 +4249,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Time!$B$73:$B$77</c:f>
+              <c:f>Time!$B$79:$B$83</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -4165,7 +4273,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Time!$G$73:$G$77</c:f>
+              <c:f>Time!$G$79:$G$83</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -4194,7 +4302,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Time!$C$89</c:f>
+              <c:f>Time!$C$95</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4229,10 +4337,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Time!$B$89:$B$97</c:f>
+              <c:f>Time!$B$95:$B$109</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -4259,42 +4367,78 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1280</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1536</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2304</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2560</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3072</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Time!$G$89:$G$97</c:f>
+              <c:f>Time!$G$95:$G$109</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>65</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>38</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>35</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>24</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>20</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>172</c:v>
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>164</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>191</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>193</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>231</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4309,11 +4453,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1852046624"/>
-        <c:axId val="-1852043904"/>
+        <c:axId val="110517632"/>
+        <c:axId val="110518024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1852046624"/>
+        <c:axId val="110517632"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -4427,12 +4571,12 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1852043904"/>
+        <c:crossAx val="110518024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1852043904"/>
+        <c:axId val="110518024"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -4546,7 +4690,7 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1852046624"/>
+        <c:crossAx val="110517632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4630,7 +4774,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="hu-HU"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -5058,11 +5202,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1852055328"/>
-        <c:axId val="-1852055872"/>
+        <c:axId val="111222744"/>
+        <c:axId val="111228232"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1852055328"/>
+        <c:axId val="111222744"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -5176,12 +5320,12 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1852055872"/>
+        <c:crossAx val="111228232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1852055872"/>
+        <c:axId val="111228232"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -5296,7 +5440,7 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1852055328"/>
+        <c:crossAx val="111222744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5380,7 +5524,7 @@
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="hu-HU"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -5991,10 +6135,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Memory!$B$45:$B$53</c:f>
+              <c:f>Memory!$B$45:$B$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -6021,42 +6165,78 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1280</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1536</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2304</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2560</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3072</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Memory!$E$45:$E$53</c:f>
+              <c:f>Memory!$E$45:$E$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>11.2783203125</c:v>
+                  <c:v>18.935546875</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19.96875</c:v>
+                  <c:v>30.724609375</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>32.681640625</c:v>
+                  <c:v>42.0283203125</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>56.9609375</c:v>
+                  <c:v>136.58203125</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>103.9814453125</c:v>
+                  <c:v>330.09375</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>308.158203125</c:v>
+                  <c:v>304.109375</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>375.4658203125</c:v>
+                  <c:v>743.4970703125</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>863.021484375</c:v>
+                  <c:v>946.603515625</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1650.6123046875</c:v>
+                  <c:v>1669.533203125</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2091.2294921875</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2454.4326171875</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3228.9697265625</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3627.3916015625</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3876.6142578125</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4227.7998046875</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6071,11 +6251,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1852046080"/>
-        <c:axId val="-1852054240"/>
+        <c:axId val="111223136"/>
+        <c:axId val="108725096"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1852046080"/>
+        <c:axId val="111223136"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -6189,12 +6369,12 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1852054240"/>
+        <c:crossAx val="108725096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1852054240"/>
+        <c:axId val="108725096"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -6309,7 +6489,7 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1852046080"/>
+        <c:crossAx val="111223136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6393,7 +6573,7 @@
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="hu-HU"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -6479,7 +6659,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Memory!$C$54</c:f>
+              <c:f>Memory!$C$60</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6514,7 +6694,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Memory!$B$54:$B$65</c:f>
+              <c:f>Memory!$B$60:$B$71</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -6559,7 +6739,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Memory!$E$54:$E$65</c:f>
+              <c:f>Memory!$E$60:$E$71</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -6609,7 +6789,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Memory!$C$66</c:f>
+              <c:f>Memory!$C$72</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6644,7 +6824,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Memory!$B$66:$B$72</c:f>
+              <c:f>Memory!$B$72:$B$78</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -6674,7 +6854,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Memory!$E$66:$E$72</c:f>
+              <c:f>Memory!$E$72:$E$78</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -6709,7 +6889,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Memory!$C$78</c:f>
+              <c:f>Memory!$C$84</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6744,7 +6924,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Memory!$B$78:$B$88</c:f>
+              <c:f>Memory!$B$84:$B$94</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -6786,7 +6966,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Memory!$E$78:$E$88</c:f>
+              <c:f>Memory!$E$84:$E$94</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -6833,7 +7013,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Memory!$C$73</c:f>
+              <c:f>Memory!$C$79</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6868,7 +7048,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Memory!$B$73:$B$77</c:f>
+              <c:f>Memory!$B$79:$B$83</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -6892,7 +7072,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Memory!$E$73:$E$77</c:f>
+              <c:f>Memory!$E$79:$E$83</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -6921,7 +7101,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Memory!$C$89</c:f>
+              <c:f>Memory!$C$95</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6956,10 +7136,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Memory!$B$89:$B$97</c:f>
+              <c:f>Memory!$B$95:$B$109</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -6986,42 +7166,78 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1280</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1536</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2304</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2560</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3072</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Memory!$E$89:$E$97</c:f>
+              <c:f>Memory!$E$95:$E$109</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>11.1865234375</c:v>
+                  <c:v>18.6181640625</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19.2880859375</c:v>
+                  <c:v>26.7197265625</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28.5595703125</c:v>
+                  <c:v>35.982421875</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>47.0234375</c:v>
+                  <c:v>54.0966796875</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>83.724609375</c:v>
+                  <c:v>91.232421875</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>156.685546875</c:v>
+                  <c:v>164.294921875</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>303.8046875</c:v>
+                  <c:v>311.4609375</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>599.650390625</c:v>
+                  <c:v>607.216796875</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1197.705078125</c:v>
+                  <c:v>1287.9794921875</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1665.271484375</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1789.921875</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2430.4619140625</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2746.7294921875</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3005.7177734375</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3606.0419921875</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7036,11 +7252,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1852052064"/>
-        <c:axId val="-1852048256"/>
+        <c:axId val="108719608"/>
+        <c:axId val="108720000"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1852052064"/>
+        <c:axId val="108719608"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -7154,12 +7370,12 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1852048256"/>
+        <c:crossAx val="108720000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1852048256"/>
+        <c:axId val="108720000"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -7273,7 +7489,7 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1852052064"/>
+        <c:crossAx val="108719608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11486,7 +11702,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-téma">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -11748,10 +11964,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H99"/>
+  <dimension ref="A1:H118"/>
   <sheetViews>
-    <sheetView topLeftCell="I20" workbookViewId="0">
-      <selection activeCell="AB37" sqref="AB37"/>
+    <sheetView tabSelected="1" topLeftCell="E7" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12799,16 +13015,16 @@
         <v>24</v>
       </c>
       <c r="D45" s="1">
-        <v>393</v>
+        <v>323</v>
       </c>
       <c r="E45" s="1">
-        <v>78</v>
+        <v>129</v>
       </c>
       <c r="F45" s="1">
-        <v>691</v>
+        <v>1728</v>
       </c>
       <c r="G45" s="1">
-        <v>60</v>
+        <v>15</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -12822,16 +13038,16 @@
         <v>24</v>
       </c>
       <c r="D46" s="1">
-        <v>183</v>
+        <v>115</v>
       </c>
       <c r="E46" s="1">
-        <v>40</v>
+        <v>115</v>
       </c>
       <c r="F46" s="1">
-        <v>914</v>
+        <v>2473</v>
       </c>
       <c r="G46" s="1">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -12845,16 +13061,16 @@
         <v>24</v>
       </c>
       <c r="D47" s="1">
-        <v>105</v>
+        <v>53</v>
       </c>
       <c r="E47" s="1">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="F47" s="1">
-        <v>1322</v>
+        <v>2119</v>
       </c>
       <c r="G47" s="1">
-        <v>30</v>
+        <v>21</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -12868,16 +13084,16 @@
         <v>24</v>
       </c>
       <c r="D48" s="1">
-        <v>153</v>
+        <v>65</v>
       </c>
       <c r="E48" s="1">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="F48" s="1">
-        <v>2698</v>
+        <v>3179</v>
       </c>
       <c r="G48" s="1">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -12891,16 +13107,16 @@
         <v>24</v>
       </c>
       <c r="D49" s="1">
-        <v>217</v>
+        <v>204</v>
       </c>
       <c r="E49" s="1">
-        <v>64</v>
+        <v>94</v>
       </c>
       <c r="F49" s="1">
-        <v>2903</v>
+        <v>4977</v>
       </c>
       <c r="G49" s="1">
-        <v>18</v>
+        <v>43</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -12914,16 +13130,16 @@
         <v>24</v>
       </c>
       <c r="D50" s="1">
-        <v>2205</v>
+        <v>234</v>
       </c>
       <c r="E50" s="1">
-        <v>491</v>
+        <v>162</v>
       </c>
       <c r="F50" s="1">
-        <v>17017</v>
+        <v>6699</v>
       </c>
       <c r="G50" s="1">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="H50"/>
     </row>
@@ -12938,16 +13154,16 @@
         <v>24</v>
       </c>
       <c r="D51" s="1">
-        <v>1034</v>
+        <v>437</v>
       </c>
       <c r="E51" s="1">
-        <v>145</v>
+        <v>342</v>
       </c>
       <c r="F51" s="1">
-        <v>19364</v>
+        <v>21218</v>
       </c>
       <c r="G51" s="1">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="H51"/>
     </row>
@@ -12962,16 +13178,16 @@
         <v>24</v>
       </c>
       <c r="D52" s="1">
-        <v>2434</v>
+        <v>1268</v>
       </c>
       <c r="E52" s="1">
-        <v>242</v>
+        <v>715</v>
       </c>
       <c r="F52" s="1">
-        <v>55916</v>
+        <v>41665</v>
       </c>
       <c r="G52" s="1">
-        <v>202</v>
+        <v>76</v>
       </c>
       <c r="H52"/>
     </row>
@@ -12986,201 +13202,201 @@
         <v>24</v>
       </c>
       <c r="D53" s="1">
-        <v>6826</v>
+        <v>3184</v>
       </c>
       <c r="E53" s="1">
-        <v>495</v>
+        <v>1497</v>
       </c>
       <c r="F53" s="1">
-        <v>187333</v>
+        <v>97030</v>
       </c>
       <c r="G53" s="1">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="H53"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="B54" s="1">
-        <v>1</v>
+        <v>1280</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="D54" s="1">
-        <v>13</v>
+        <v>6112</v>
       </c>
       <c r="E54" s="1">
-        <v>21</v>
+        <v>1899</v>
       </c>
       <c r="F54" s="1">
-        <v>124</v>
+        <v>162317</v>
       </c>
       <c r="G54" s="1">
-        <v>93</v>
+        <v>121</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>0</v>
+      </c>
+      <c r="B55" s="1">
+        <v>1536</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D55" s="1">
+        <v>5613</v>
+      </c>
+      <c r="E55" s="1">
+        <v>2194</v>
+      </c>
+      <c r="F55" s="1">
+        <v>138240</v>
+      </c>
+      <c r="G55" s="1">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>0</v>
+      </c>
+      <c r="B56" s="1">
+        <v>2048</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D56" s="1">
+        <v>11732</v>
+      </c>
+      <c r="E56" s="1">
+        <v>3266</v>
+      </c>
+      <c r="F56" s="1">
+        <v>337698</v>
+      </c>
+      <c r="G56" s="1">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>0</v>
+      </c>
+      <c r="B57" s="1">
+        <v>2304</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D57" s="1">
+        <v>20035</v>
+      </c>
+      <c r="E57" s="1">
+        <v>3651</v>
+      </c>
+      <c r="F57" s="1">
+        <v>379205</v>
+      </c>
+      <c r="G57" s="1">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>0</v>
+      </c>
+      <c r="B58" s="1">
+        <v>2560</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D58" s="1">
+        <v>15271</v>
+      </c>
+      <c r="E58" s="1">
+        <v>4009</v>
+      </c>
+      <c r="F58" s="1">
+        <v>351245</v>
+      </c>
+      <c r="G58" s="1">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>0</v>
+      </c>
+      <c r="B59" s="1">
+        <v>3072</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D59" s="1">
+        <v>33055</v>
+      </c>
+      <c r="E59" s="1">
+        <v>4534</v>
+      </c>
+      <c r="F59" s="1">
+        <v>214484</v>
+      </c>
+      <c r="G59" s="1">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>18</v>
       </c>
-      <c r="B55" s="1">
-        <v>8</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D55" s="1">
-        <v>34</v>
-      </c>
-      <c r="E55" s="1">
-        <v>24</v>
-      </c>
-      <c r="F55" s="1">
-        <v>169</v>
-      </c>
-      <c r="G55" s="1">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B56" s="1">
-        <v>16</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D56" s="1">
-        <v>818</v>
-      </c>
-      <c r="E56" s="1">
-        <v>57</v>
-      </c>
-      <c r="F56" s="1">
-        <v>1129</v>
-      </c>
-      <c r="G56" s="1">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B57" s="1">
-        <v>32</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D57" s="1">
-        <v>148</v>
-      </c>
-      <c r="E57" s="1">
-        <v>14</v>
-      </c>
-      <c r="F57" s="1">
-        <v>387</v>
-      </c>
-      <c r="G57" s="1">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B58" s="1">
-        <v>64</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D58" s="1">
-        <v>146</v>
-      </c>
-      <c r="E58" s="1">
-        <v>17</v>
-      </c>
-      <c r="F58" s="1">
-        <v>701</v>
-      </c>
-      <c r="G58" s="1">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B59" s="1">
-        <v>128</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D59" s="1">
-        <v>243</v>
-      </c>
-      <c r="E59" s="1">
-        <v>29</v>
-      </c>
-      <c r="F59" s="1">
-        <v>1230</v>
-      </c>
-      <c r="G59" s="1">
-        <v>1269</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="B60" s="1">
-        <v>256</v>
+        <v>1</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D60" s="1">
-        <v>596</v>
+        <v>13</v>
       </c>
       <c r="E60" s="1">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="F60" s="1">
-        <v>2268</v>
+        <v>124</v>
       </c>
       <c r="G60" s="1">
-        <v>2423</v>
+        <v>93</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="4" t="s">
+      <c r="A61" t="s">
         <v>18</v>
       </c>
       <c r="B61" s="1">
-        <v>512</v>
+        <v>8</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D61" s="1">
-        <v>2933</v>
+        <v>34</v>
       </c>
       <c r="E61" s="1">
-        <v>403</v>
+        <v>24</v>
       </c>
       <c r="F61" s="1">
-        <v>6250</v>
+        <v>169</v>
       </c>
       <c r="G61" s="1">
-        <v>4348</v>
+        <v>152</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
@@ -13188,137 +13404,137 @@
         <v>18</v>
       </c>
       <c r="B62" s="1">
-        <v>1024</v>
+        <v>16</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D62" s="1">
-        <v>5420</v>
+        <v>818</v>
       </c>
       <c r="E62" s="1">
-        <v>324</v>
+        <v>57</v>
       </c>
       <c r="F62" s="1">
-        <v>7616</v>
+        <v>1129</v>
       </c>
       <c r="G62" s="1">
-        <v>9909</v>
+        <v>459</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+      <c r="A63" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B63" s="1">
-        <v>1280</v>
+        <v>32</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D63" s="1">
-        <v>10060</v>
+        <v>148</v>
       </c>
       <c r="E63" s="1">
-        <v>470</v>
+        <v>14</v>
       </c>
       <c r="F63" s="1">
-        <v>11177</v>
+        <v>387</v>
       </c>
       <c r="G63" s="1">
-        <v>10286</v>
+        <v>344</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+      <c r="A64" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B64" s="1">
-        <v>1536</v>
+        <v>64</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D64" s="1">
-        <v>11887</v>
+        <v>146</v>
       </c>
       <c r="E64" s="1">
-        <v>361</v>
+        <v>17</v>
       </c>
       <c r="F64" s="1">
-        <v>12126</v>
+        <v>701</v>
       </c>
       <c r="G64" s="1">
-        <v>13776</v>
+        <v>442</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+      <c r="A65" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B65" s="1">
-        <v>2048</v>
+        <v>128</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D65" s="1">
-        <v>11487</v>
+        <v>243</v>
       </c>
       <c r="E65" s="1">
-        <v>513</v>
+        <v>29</v>
       </c>
       <c r="F65" s="1">
-        <v>13213</v>
+        <v>1230</v>
       </c>
       <c r="G65" s="1">
-        <v>14713</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+      <c r="A66" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B66" s="1">
-        <v>1</v>
+        <v>256</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D66" s="1">
-        <v>16</v>
+        <v>596</v>
       </c>
       <c r="E66" s="1">
-        <v>20</v>
+        <v>57</v>
       </c>
       <c r="F66" s="1">
-        <v>93</v>
+        <v>2268</v>
       </c>
       <c r="G66" s="1">
-        <v>81</v>
+        <v>2423</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+      <c r="A67" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B67" s="1">
-        <v>8</v>
+        <v>512</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D67" s="1">
-        <v>50</v>
+        <v>2933</v>
       </c>
       <c r="E67" s="1">
-        <v>29</v>
+        <v>403</v>
       </c>
       <c r="F67" s="1">
-        <v>188</v>
+        <v>6250</v>
       </c>
       <c r="G67" s="1">
-        <v>218</v>
+        <v>4348</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
@@ -13326,116 +13542,116 @@
         <v>18</v>
       </c>
       <c r="B68" s="1">
-        <v>16</v>
+        <v>1024</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D68" s="1">
-        <v>685</v>
+        <v>5420</v>
       </c>
       <c r="E68" s="1">
-        <v>88</v>
+        <v>324</v>
       </c>
       <c r="F68" s="1">
-        <v>1152</v>
+        <v>7616</v>
       </c>
       <c r="G68" s="1">
-        <v>667</v>
+        <v>9909</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69" s="4" t="s">
+      <c r="A69" t="s">
         <v>18</v>
       </c>
       <c r="B69" s="1">
-        <v>32</v>
+        <v>1280</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D69" s="1">
-        <v>204</v>
+        <v>10060</v>
       </c>
       <c r="E69" s="1">
-        <v>27</v>
+        <v>470</v>
       </c>
       <c r="F69" s="1">
-        <v>822</v>
+        <v>11177</v>
       </c>
       <c r="G69" s="1">
-        <v>1053</v>
+        <v>10286</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" s="4" t="s">
+      <c r="A70" t="s">
         <v>18</v>
       </c>
       <c r="B70" s="1">
-        <v>64</v>
+        <v>1536</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D70" s="1">
-        <v>167</v>
+        <v>11887</v>
       </c>
       <c r="E70" s="1">
-        <v>35</v>
+        <v>361</v>
       </c>
       <c r="F70" s="1">
-        <v>4091</v>
+        <v>12126</v>
       </c>
       <c r="G70" s="1">
-        <v>3667</v>
+        <v>13776</v>
       </c>
       <c r="H70"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" s="4" t="s">
+      <c r="A71" t="s">
         <v>18</v>
       </c>
       <c r="B71" s="1">
-        <v>128</v>
+        <v>2048</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D71" s="1">
-        <v>271</v>
+        <v>11487</v>
       </c>
       <c r="E71" s="1">
-        <v>27</v>
+        <v>513</v>
       </c>
       <c r="F71" s="1">
-        <v>17054</v>
+        <v>13213</v>
       </c>
       <c r="G71" s="1">
-        <v>14678</v>
+        <v>14713</v>
       </c>
       <c r="H71"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A72" s="4" t="s">
+      <c r="A72" t="s">
         <v>18</v>
       </c>
       <c r="B72" s="1">
-        <v>256</v>
+        <v>1</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D72" s="1">
-        <v>473</v>
+        <v>16</v>
       </c>
       <c r="E72" s="1">
-        <v>62</v>
+        <v>20</v>
       </c>
       <c r="F72" s="1">
-        <v>77935</v>
+        <v>93</v>
       </c>
       <c r="G72" s="1">
-        <v>71400</v>
+        <v>81</v>
       </c>
       <c r="H72"/>
     </row>
@@ -13444,46 +13660,46 @@
         <v>18</v>
       </c>
       <c r="B73" s="1">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D73" s="1">
-        <v>297</v>
+        <v>50</v>
       </c>
       <c r="E73" s="1">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="F73" s="1">
-        <v>141</v>
+        <v>188</v>
       </c>
       <c r="G73" s="1">
-        <v>131</v>
+        <v>218</v>
       </c>
       <c r="H73"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+      <c r="A74" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B74" s="1">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D74" s="1">
-        <v>127</v>
+        <v>685</v>
       </c>
       <c r="E74" s="1">
-        <v>34</v>
+        <v>88</v>
       </c>
       <c r="F74" s="1">
-        <v>727</v>
+        <v>1152</v>
       </c>
       <c r="G74" s="1">
-        <v>675</v>
+        <v>667</v>
       </c>
       <c r="H74"/>
     </row>
@@ -13492,22 +13708,22 @@
         <v>18</v>
       </c>
       <c r="B75" s="1">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D75" s="1">
-        <v>672</v>
+        <v>204</v>
       </c>
       <c r="E75" s="1">
-        <v>86</v>
+        <v>27</v>
       </c>
       <c r="F75" s="1">
-        <v>3615</v>
+        <v>822</v>
       </c>
       <c r="G75" s="1">
-        <v>3009</v>
+        <v>1053</v>
       </c>
       <c r="H75"/>
     </row>
@@ -13516,22 +13732,22 @@
         <v>18</v>
       </c>
       <c r="B76" s="1">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D76" s="1">
-        <v>184</v>
+        <v>167</v>
       </c>
       <c r="E76" s="1">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="F76" s="1">
-        <v>7654</v>
+        <v>4091</v>
       </c>
       <c r="G76" s="1">
-        <v>7306</v>
+        <v>3667</v>
       </c>
       <c r="H76"/>
     </row>
@@ -13540,46 +13756,46 @@
         <v>18</v>
       </c>
       <c r="B77" s="1">
-        <v>64</v>
+        <v>128</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D77" s="1">
-        <v>142</v>
+        <v>271</v>
       </c>
       <c r="E77" s="1">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="F77" s="1">
-        <v>39978</v>
+        <v>17054</v>
       </c>
       <c r="G77" s="1">
-        <v>44263</v>
+        <v>14678</v>
       </c>
       <c r="H77"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
+      <c r="A78" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B78" s="1">
-        <v>1</v>
+        <v>256</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D78" s="1">
-        <v>8</v>
+        <v>473</v>
       </c>
       <c r="E78" s="1">
-        <v>12</v>
+        <v>62</v>
       </c>
       <c r="F78" s="1">
-        <v>419</v>
+        <v>77935</v>
       </c>
       <c r="G78" s="1">
-        <v>31</v>
+        <v>71400</v>
       </c>
       <c r="H78"/>
     </row>
@@ -13588,46 +13804,46 @@
         <v>18</v>
       </c>
       <c r="B79" s="1">
+        <v>1</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D79" s="1">
+        <v>297</v>
+      </c>
+      <c r="E79" s="1">
+        <v>65</v>
+      </c>
+      <c r="F79" s="1">
+        <v>141</v>
+      </c>
+      <c r="G79" s="1">
+        <v>131</v>
+      </c>
+      <c r="H79"/>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>18</v>
+      </c>
+      <c r="B80" s="1">
         <v>8</v>
       </c>
-      <c r="C79" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D79" s="1">
-        <v>24</v>
-      </c>
-      <c r="E79" s="1">
-        <v>17</v>
-      </c>
-      <c r="F79" s="1">
-        <v>553</v>
-      </c>
-      <c r="G79" s="1">
-        <v>15</v>
-      </c>
-      <c r="H79"/>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A80" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B80" s="1">
-        <v>16</v>
-      </c>
       <c r="C80" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D80" s="1">
-        <v>55</v>
+        <v>127</v>
       </c>
       <c r="E80" s="1">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="F80" s="1">
-        <v>2028</v>
+        <v>727</v>
       </c>
       <c r="G80" s="1">
-        <v>16</v>
+        <v>675</v>
       </c>
       <c r="H80"/>
     </row>
@@ -13636,22 +13852,22 @@
         <v>18</v>
       </c>
       <c r="B81" s="1">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D81" s="1">
-        <v>48</v>
+        <v>672</v>
       </c>
       <c r="E81" s="1">
-        <v>7</v>
+        <v>86</v>
       </c>
       <c r="F81" s="1">
-        <v>1552</v>
+        <v>3615</v>
       </c>
       <c r="G81" s="1">
-        <v>2</v>
+        <v>3009</v>
       </c>
       <c r="H81"/>
     </row>
@@ -13660,22 +13876,22 @@
         <v>18</v>
       </c>
       <c r="B82" s="1">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D82" s="1">
-        <v>90</v>
+        <v>184</v>
       </c>
       <c r="E82" s="1">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="F82" s="1">
-        <v>2753</v>
+        <v>7654</v>
       </c>
       <c r="G82" s="1">
-        <v>4</v>
+        <v>7306</v>
       </c>
       <c r="H82"/>
     </row>
@@ -13684,70 +13900,70 @@
         <v>18</v>
       </c>
       <c r="B83" s="1">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D83" s="1">
-        <v>264</v>
+        <v>142</v>
       </c>
       <c r="E83" s="1">
         <v>23</v>
       </c>
       <c r="F83" s="1">
-        <v>7032</v>
+        <v>39978</v>
       </c>
       <c r="G83" s="1">
-        <v>6</v>
+        <v>44263</v>
       </c>
       <c r="H83"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A84" s="4" t="s">
+      <c r="A84" t="s">
         <v>18</v>
       </c>
       <c r="B84" s="1">
-        <v>256</v>
+        <v>1</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D84" s="1">
-        <v>405</v>
+        <v>8</v>
       </c>
       <c r="E84" s="1">
-        <v>62</v>
+        <v>12</v>
       </c>
       <c r="F84" s="1">
-        <v>10925</v>
+        <v>419</v>
       </c>
       <c r="G84" s="1">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="H84"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A85" s="4" t="s">
+      <c r="A85" t="s">
         <v>18</v>
       </c>
       <c r="B85" s="1">
-        <v>512</v>
+        <v>8</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D85" s="1">
-        <v>2005</v>
+        <v>24</v>
       </c>
       <c r="E85" s="1">
-        <v>121</v>
+        <v>17</v>
       </c>
       <c r="F85" s="1">
-        <v>36657</v>
+        <v>553</v>
       </c>
       <c r="G85" s="1">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="H85"/>
     </row>
@@ -13756,166 +13972,166 @@
         <v>18</v>
       </c>
       <c r="B86" s="1">
-        <v>1024</v>
+        <v>16</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D86" s="1">
-        <v>4689</v>
+        <v>55</v>
       </c>
       <c r="E86" s="1">
-        <v>310</v>
+        <v>5</v>
       </c>
       <c r="F86" s="1">
-        <v>109136</v>
+        <v>2028</v>
       </c>
       <c r="G86" s="1">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H86"/>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+      <c r="A87" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B87" s="1">
-        <v>1280</v>
+        <v>32</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D87" s="1">
-        <v>6689</v>
+        <v>48</v>
       </c>
       <c r="E87" s="1">
-        <v>296</v>
+        <v>7</v>
       </c>
       <c r="F87" s="1">
-        <v>55550</v>
+        <v>1552</v>
       </c>
       <c r="G87" s="1">
-        <v>53</v>
+        <v>2</v>
       </c>
       <c r="H87"/>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+      <c r="A88" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B88" s="1">
-        <v>1536</v>
+        <v>64</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D88" s="1">
-        <v>8710</v>
+        <v>90</v>
       </c>
       <c r="E88" s="1">
-        <v>347</v>
+        <v>12</v>
       </c>
       <c r="F88" s="1">
-        <v>73343</v>
+        <v>2753</v>
       </c>
       <c r="G88" s="1">
-        <v>52</v>
+        <v>4</v>
       </c>
       <c r="H88"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
+      <c r="A89" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B89" s="1">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="D89" s="1">
-        <v>416</v>
+        <v>264</v>
       </c>
       <c r="E89" s="1">
-        <v>101</v>
+        <v>23</v>
       </c>
       <c r="F89" s="1">
-        <v>638</v>
+        <v>7032</v>
       </c>
       <c r="G89" s="1">
-        <v>65</v>
+        <v>6</v>
       </c>
       <c r="H89"/>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
+      <c r="A90" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B90" s="1">
-        <v>8</v>
+        <v>256</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="D90" s="1">
-        <v>161</v>
+        <v>405</v>
       </c>
       <c r="E90" s="1">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="F90" s="1">
-        <v>967</v>
+        <v>10925</v>
       </c>
       <c r="G90" s="1">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="H90"/>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
+      <c r="A91" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B91" s="1">
-        <v>16</v>
+        <v>512</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="D91" s="1">
-        <v>112</v>
+        <v>2005</v>
       </c>
       <c r="E91" s="1">
-        <v>47</v>
+        <v>121</v>
       </c>
       <c r="F91" s="1">
-        <v>894</v>
+        <v>36657</v>
       </c>
       <c r="G91" s="1">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="H91"/>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
+      <c r="A92" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B92" s="1">
-        <v>32</v>
+        <v>1024</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="D92" s="1">
-        <v>138</v>
+        <v>4689</v>
       </c>
       <c r="E92" s="1">
-        <v>78</v>
+        <v>310</v>
       </c>
       <c r="F92" s="1">
-        <v>1178</v>
+        <v>109136</v>
       </c>
       <c r="G92" s="1">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="H92"/>
     </row>
@@ -13924,22 +14140,22 @@
         <v>18</v>
       </c>
       <c r="B93" s="1">
-        <v>64</v>
+        <v>1280</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="D93" s="1">
-        <v>259</v>
+        <v>6689</v>
       </c>
       <c r="E93" s="1">
-        <v>84</v>
+        <v>296</v>
       </c>
       <c r="F93" s="1">
-        <v>3509</v>
+        <v>55550</v>
       </c>
       <c r="G93" s="1">
-        <v>9</v>
+        <v>53</v>
       </c>
       <c r="H93"/>
     </row>
@@ -13948,22 +14164,22 @@
         <v>18</v>
       </c>
       <c r="B94" s="1">
-        <v>128</v>
+        <v>1536</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="D94" s="1">
-        <v>437</v>
+        <v>8710</v>
       </c>
       <c r="E94" s="1">
-        <v>126</v>
+        <v>347</v>
       </c>
       <c r="F94" s="1">
-        <v>3560</v>
+        <v>73343</v>
       </c>
       <c r="G94" s="1">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="H94"/>
     </row>
@@ -13972,22 +14188,22 @@
         <v>18</v>
       </c>
       <c r="B95" s="1">
-        <v>256</v>
+        <v>1</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D95" s="1">
-        <v>812</v>
+        <v>267</v>
       </c>
       <c r="E95" s="1">
-        <v>163</v>
+        <v>132</v>
       </c>
       <c r="F95" s="1">
-        <v>6063</v>
+        <v>1669</v>
       </c>
       <c r="G95" s="1">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="H95"/>
     </row>
@@ -13996,22 +14212,22 @@
         <v>18</v>
       </c>
       <c r="B96" s="1">
-        <v>512</v>
+        <v>8</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D96" s="1">
-        <v>2016</v>
+        <v>115</v>
       </c>
       <c r="E96" s="1">
-        <v>204</v>
+        <v>57</v>
       </c>
       <c r="F96" s="1">
-        <v>18451</v>
+        <v>1867</v>
       </c>
       <c r="G96" s="1">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="H96"/>
     </row>
@@ -14020,30 +14236,327 @@
         <v>18</v>
       </c>
       <c r="B97" s="1">
-        <v>1024</v>
+        <v>16</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D97" s="1">
-        <v>6791</v>
+        <v>58</v>
       </c>
       <c r="E97" s="1">
-        <v>399</v>
+        <v>51</v>
       </c>
       <c r="F97" s="1">
-        <v>32176</v>
+        <v>1905</v>
       </c>
       <c r="G97" s="1">
-        <v>172</v>
+        <v>13</v>
       </c>
       <c r="H97"/>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A98"/>
+      <c r="A98" t="s">
+        <v>18</v>
+      </c>
+      <c r="B98" s="1">
+        <v>32</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D98" s="1">
+        <v>73</v>
+      </c>
+      <c r="E98" s="1">
+        <v>56</v>
+      </c>
+      <c r="F98" s="1">
+        <v>2020</v>
+      </c>
+      <c r="G98" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A99"/>
+      <c r="A99" t="s">
+        <v>18</v>
+      </c>
+      <c r="B99" s="1">
+        <v>64</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D99" s="1">
+        <v>98</v>
+      </c>
+      <c r="E99" s="1">
+        <v>86</v>
+      </c>
+      <c r="F99" s="1">
+        <v>2927</v>
+      </c>
+      <c r="G99" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>18</v>
+      </c>
+      <c r="B100" s="1">
+        <v>128</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D100" s="1">
+        <v>208</v>
+      </c>
+      <c r="E100" s="1">
+        <v>143</v>
+      </c>
+      <c r="F100" s="1">
+        <v>4119</v>
+      </c>
+      <c r="G100" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>18</v>
+      </c>
+      <c r="B101" s="1">
+        <v>256</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D101" s="1">
+        <v>415</v>
+      </c>
+      <c r="E101" s="1">
+        <v>304</v>
+      </c>
+      <c r="F101" s="1">
+        <v>5879</v>
+      </c>
+      <c r="G101" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>18</v>
+      </c>
+      <c r="B102" s="1">
+        <v>512</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D102" s="1">
+        <v>1422</v>
+      </c>
+      <c r="E102" s="1">
+        <v>604</v>
+      </c>
+      <c r="F102" s="1">
+        <v>13580</v>
+      </c>
+      <c r="G102" s="1">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>18</v>
+      </c>
+      <c r="B103" s="1">
+        <v>1024</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D103" s="1">
+        <v>5044</v>
+      </c>
+      <c r="E103" s="1">
+        <v>1330</v>
+      </c>
+      <c r="F103" s="1">
+        <v>27465</v>
+      </c>
+      <c r="G103" s="1">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>18</v>
+      </c>
+      <c r="B104" s="1">
+        <v>1280</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D104" s="1">
+        <v>7970</v>
+      </c>
+      <c r="E104" s="1">
+        <v>1669</v>
+      </c>
+      <c r="F104" s="1">
+        <v>31295</v>
+      </c>
+      <c r="G104" s="1">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>18</v>
+      </c>
+      <c r="B105" s="1">
+        <v>1536</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D105" s="1">
+        <v>10458</v>
+      </c>
+      <c r="E105" s="1">
+        <v>1928</v>
+      </c>
+      <c r="F105" s="1">
+        <v>43129</v>
+      </c>
+      <c r="G105" s="1">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>18</v>
+      </c>
+      <c r="B106" s="1">
+        <v>2048</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D106" s="1">
+        <v>18189</v>
+      </c>
+      <c r="E106" s="1">
+        <v>2865</v>
+      </c>
+      <c r="F106" s="1">
+        <v>51263</v>
+      </c>
+      <c r="G106" s="1">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>18</v>
+      </c>
+      <c r="B107" s="1">
+        <v>2304</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D107" s="1">
+        <v>18909</v>
+      </c>
+      <c r="E107" s="1">
+        <v>3220</v>
+      </c>
+      <c r="F107" s="1">
+        <v>72592</v>
+      </c>
+      <c r="G107" s="1">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>18</v>
+      </c>
+      <c r="B108" s="1">
+        <v>2560</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D108" s="1">
+        <v>21812</v>
+      </c>
+      <c r="E108" s="1">
+        <v>3535</v>
+      </c>
+      <c r="F108" s="1">
+        <v>86368</v>
+      </c>
+      <c r="G108" s="1">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>18</v>
+      </c>
+      <c r="B109" s="1">
+        <v>3072</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D109" s="1">
+        <v>38036</v>
+      </c>
+      <c r="E109" s="1">
+        <v>4358</v>
+      </c>
+      <c r="F109" s="1">
+        <v>86160</v>
+      </c>
+      <c r="G109" s="1">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A110"/>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A111"/>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A112"/>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113"/>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114"/>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115"/>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116"/>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117"/>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118"/>
     </row>
   </sheetData>
   <sortState ref="A2:G78">
@@ -16894,10 +17407,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G97"/>
+  <dimension ref="A1:G109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
-      <selection activeCell="C100" sqref="C100"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="N60" sqref="N60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17812,13 +18325,13 @@
         <v>24</v>
       </c>
       <c r="D45" s="1">
-        <v>71906</v>
+        <v>285691</v>
       </c>
       <c r="E45" s="1">
-        <v>11.2783203125</v>
+        <v>18.935546875</v>
       </c>
       <c r="F45" s="1">
-        <v>11646</v>
+        <v>19083</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -17832,13 +18345,13 @@
         <v>24</v>
       </c>
       <c r="D46" s="1">
-        <v>13553</v>
+        <v>94389</v>
       </c>
       <c r="E46" s="1">
-        <v>19.96875</v>
+        <v>30.724609375</v>
       </c>
       <c r="F46" s="1">
-        <v>20741</v>
+        <v>31775</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -17852,13 +18365,13 @@
         <v>24</v>
       </c>
       <c r="D47" s="1">
-        <v>26016</v>
+        <v>37073</v>
       </c>
       <c r="E47" s="1">
-        <v>32.681640625</v>
+        <v>42.0283203125</v>
       </c>
       <c r="F47" s="1">
-        <v>33992</v>
+        <v>43555</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -17872,13 +18385,13 @@
         <v>24</v>
       </c>
       <c r="D48" s="1">
-        <v>65134</v>
+        <v>53688</v>
       </c>
       <c r="E48" s="1">
-        <v>56.9609375</v>
+        <v>136.58203125</v>
       </c>
       <c r="F48" s="1">
-        <v>59280</v>
+        <v>581836</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -17892,13 +18405,13 @@
         <v>24</v>
       </c>
       <c r="D49" s="1">
-        <v>79144</v>
+        <v>381950</v>
       </c>
       <c r="E49" s="1">
-        <v>103.9814453125</v>
+        <v>330.09375</v>
       </c>
       <c r="F49" s="1">
-        <v>108226</v>
+        <v>266470</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -17912,13 +18425,13 @@
         <v>24</v>
       </c>
       <c r="D50" s="1">
-        <v>90273</v>
+        <v>378981</v>
       </c>
       <c r="E50" s="1">
-        <v>308.158203125</v>
+        <v>304.109375</v>
       </c>
       <c r="F50" s="1">
-        <v>219584</v>
+        <v>314957</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -17932,13 +18445,13 @@
         <v>24</v>
       </c>
       <c r="D51" s="1">
-        <v>297735</v>
+        <v>347392</v>
       </c>
       <c r="E51" s="1">
-        <v>375.4658203125</v>
+        <v>743.4970703125</v>
       </c>
       <c r="F51" s="1">
-        <v>431109</v>
+        <v>503024</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -17952,13 +18465,13 @@
         <v>24</v>
       </c>
       <c r="D52" s="1">
-        <v>546005</v>
+        <v>631603</v>
       </c>
       <c r="E52" s="1">
-        <v>863.021484375</v>
+        <v>946.603515625</v>
       </c>
       <c r="F52" s="1">
-        <v>897255</v>
+        <v>891536</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -17972,133 +18485,133 @@
         <v>24</v>
       </c>
       <c r="D53" s="1">
-        <v>1214117</v>
+        <v>1198548</v>
       </c>
       <c r="E53" s="1">
-        <v>1650.6123046875</v>
+        <v>1669.533203125</v>
       </c>
       <c r="F53" s="1">
-        <v>1717042</v>
+        <v>1692386</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="B54" s="1">
-        <v>1</v>
+        <v>1280</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="D54" s="1">
-        <v>30429</v>
+        <v>2227414</v>
       </c>
       <c r="E54" s="1">
-        <v>108.978515625</v>
+        <v>2091.2294921875</v>
       </c>
       <c r="F54" s="1">
-        <v>33246</v>
+        <v>2154516</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="B55" s="1">
-        <v>8</v>
+        <v>1536</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="D55" s="1">
-        <v>33560</v>
+        <v>2801773</v>
       </c>
       <c r="E55" s="1">
-        <v>39.1572265625</v>
+        <v>2454.4326171875</v>
       </c>
       <c r="F55" s="1">
-        <v>41177</v>
+        <v>2510605</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="B56" s="1">
-        <v>16</v>
+        <v>2048</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="D56" s="1">
-        <v>148702</v>
+        <v>3252535</v>
       </c>
       <c r="E56" s="1">
-        <v>32.658203125</v>
+        <v>3228.9697265625</v>
       </c>
       <c r="F56" s="1">
-        <v>35259</v>
+        <v>3371102</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="B57" s="1">
-        <v>32</v>
+        <v>2304</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="D57" s="1">
-        <v>33656</v>
+        <v>4305222</v>
       </c>
       <c r="E57" s="1">
-        <v>48.17578125</v>
+        <v>3627.3916015625</v>
       </c>
       <c r="F57" s="1">
-        <v>52943</v>
+        <v>3772061</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="B58" s="1">
-        <v>64</v>
+        <v>2560</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="D58" s="1">
-        <v>50412</v>
+        <v>4859620</v>
       </c>
       <c r="E58" s="1">
-        <v>79.892578125</v>
+        <v>3876.6142578125</v>
       </c>
       <c r="F58" s="1">
-        <v>141265</v>
+        <v>4034759</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="B59" s="1">
-        <v>128</v>
+        <v>3072</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="D59" s="1">
-        <v>84589</v>
+        <v>5207588</v>
       </c>
       <c r="E59" s="1">
-        <v>143.466796875</v>
+        <v>4227.7998046875</v>
       </c>
       <c r="F59" s="1">
-        <v>160680</v>
+        <v>4386454</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -18106,19 +18619,19 @@
         <v>18</v>
       </c>
       <c r="B60" s="1">
-        <v>256</v>
+        <v>1</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D60" s="1">
-        <v>151603</v>
+        <v>30429</v>
       </c>
       <c r="E60" s="1">
-        <v>270.912109375</v>
+        <v>108.978515625</v>
       </c>
       <c r="F60" s="1">
-        <v>304740</v>
+        <v>33246</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -18126,19 +18639,19 @@
         <v>18</v>
       </c>
       <c r="B61" s="1">
-        <v>512</v>
+        <v>8</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D61" s="1">
-        <v>203529</v>
+        <v>33560</v>
       </c>
       <c r="E61" s="1">
-        <v>541.1083984375</v>
+        <v>39.1572265625</v>
       </c>
       <c r="F61" s="1">
-        <v>608139</v>
+        <v>41177</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -18146,19 +18659,19 @@
         <v>18</v>
       </c>
       <c r="B62" s="1">
-        <v>1024</v>
+        <v>16</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D62" s="1">
-        <v>593116</v>
+        <v>148702</v>
       </c>
       <c r="E62" s="1">
-        <v>1071.5068359375</v>
+        <v>32.658203125</v>
       </c>
       <c r="F62" s="1">
-        <v>1204256</v>
+        <v>35259</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -18166,19 +18679,19 @@
         <v>18</v>
       </c>
       <c r="B63" s="1">
-        <v>1280</v>
+        <v>32</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D63" s="1">
-        <v>331918</v>
+        <v>33656</v>
       </c>
       <c r="E63" s="1">
-        <v>1347.2314453125</v>
+        <v>48.17578125</v>
       </c>
       <c r="F63" s="1">
-        <v>1513187</v>
+        <v>52943</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -18186,19 +18699,19 @@
         <v>18</v>
       </c>
       <c r="B64" s="1">
-        <v>1536</v>
+        <v>64</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D64" s="1">
-        <v>1201996</v>
+        <v>50412</v>
       </c>
       <c r="E64" s="1">
-        <v>1607.919921875</v>
+        <v>79.892578125</v>
       </c>
       <c r="F64" s="1">
-        <v>1807929</v>
+        <v>141265</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -18206,19 +18719,19 @@
         <v>18</v>
       </c>
       <c r="B65" s="1">
-        <v>2048</v>
+        <v>128</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D65" s="1">
-        <v>1460368</v>
+        <v>84589</v>
       </c>
       <c r="E65" s="1">
-        <v>2176.1015625</v>
+        <v>143.466796875</v>
       </c>
       <c r="F65" s="1">
-        <v>2441838</v>
+        <v>160680</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -18226,19 +18739,19 @@
         <v>18</v>
       </c>
       <c r="B66" s="1">
-        <v>1</v>
+        <v>256</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D66" s="1">
-        <v>23010</v>
+        <v>151603</v>
       </c>
       <c r="E66" s="1">
-        <v>22.7421875</v>
+        <v>270.912109375</v>
       </c>
       <c r="F66" s="1">
-        <v>23335</v>
+        <v>304740</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -18246,19 +18759,19 @@
         <v>18</v>
       </c>
       <c r="B67" s="1">
-        <v>8</v>
+        <v>512</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D67" s="1">
-        <v>25559</v>
+        <v>203529</v>
       </c>
       <c r="E67" s="1">
-        <v>24.912109375</v>
+        <v>541.1083984375</v>
       </c>
       <c r="F67" s="1">
-        <v>25737</v>
+        <v>608139</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -18266,19 +18779,19 @@
         <v>18</v>
       </c>
       <c r="B68" s="1">
-        <v>16</v>
+        <v>1024</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D68" s="1">
-        <v>207334</v>
+        <v>593116</v>
       </c>
       <c r="E68" s="1">
-        <v>20.544921875</v>
+        <v>1071.5068359375</v>
       </c>
       <c r="F68" s="1">
-        <v>21410</v>
+        <v>1204256</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -18286,19 +18799,19 @@
         <v>18</v>
       </c>
       <c r="B69" s="1">
-        <v>32</v>
+        <v>1280</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D69" s="1">
-        <v>34281</v>
+        <v>331918</v>
       </c>
       <c r="E69" s="1">
-        <v>25.4189453125</v>
+        <v>1347.2314453125</v>
       </c>
       <c r="F69" s="1">
-        <v>26807</v>
+        <v>1513187</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -18306,19 +18819,19 @@
         <v>18</v>
       </c>
       <c r="B70" s="1">
-        <v>64</v>
+        <v>1536</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D70" s="1">
-        <v>51744</v>
+        <v>1201996</v>
       </c>
       <c r="E70" s="1">
-        <v>164.5615234375</v>
+        <v>1607.919921875</v>
       </c>
       <c r="F70" s="1">
-        <v>38259</v>
+        <v>1807929</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -18326,19 +18839,19 @@
         <v>18</v>
       </c>
       <c r="B71" s="1">
-        <v>128</v>
+        <v>2048</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D71" s="1">
-        <v>87376</v>
+        <v>1460368</v>
       </c>
       <c r="E71" s="1">
-        <v>55.583984375</v>
+        <v>2176.1015625</v>
       </c>
       <c r="F71" s="1">
-        <v>59899</v>
+        <v>2441838</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -18346,19 +18859,19 @@
         <v>18</v>
       </c>
       <c r="B72" s="1">
-        <v>256</v>
+        <v>1</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D72" s="1">
-        <v>157235</v>
+        <v>23010</v>
       </c>
       <c r="E72" s="1">
-        <v>114.1259765625</v>
+        <v>22.7421875</v>
       </c>
       <c r="F72" s="1">
-        <v>103303</v>
+        <v>23335</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -18366,19 +18879,19 @@
         <v>18</v>
       </c>
       <c r="B73" s="1">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D73" s="1">
-        <v>205355</v>
+        <v>25559</v>
       </c>
       <c r="E73" s="1">
-        <v>15.8818359375</v>
+        <v>24.912109375</v>
       </c>
       <c r="F73" s="1">
-        <v>16218</v>
+        <v>25737</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -18386,19 +18899,19 @@
         <v>18</v>
       </c>
       <c r="B74" s="1">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D74" s="1">
-        <v>18449</v>
+        <v>207334</v>
       </c>
       <c r="E74" s="1">
-        <v>17.857421875</v>
+        <v>20.544921875</v>
       </c>
       <c r="F74" s="1">
-        <v>18299</v>
+        <v>21410</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -18406,19 +18919,19 @@
         <v>18</v>
       </c>
       <c r="B75" s="1">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D75" s="1">
-        <v>207347</v>
+        <v>34281</v>
       </c>
       <c r="E75" s="1">
-        <v>20.181640625</v>
+        <v>25.4189453125</v>
       </c>
       <c r="F75" s="1">
-        <v>20638</v>
+        <v>26807</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -18426,19 +18939,19 @@
         <v>18</v>
       </c>
       <c r="B76" s="1">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D76" s="1">
-        <v>33487</v>
+        <v>51744</v>
       </c>
       <c r="E76" s="1">
-        <v>25.259765625</v>
+        <v>164.5615234375</v>
       </c>
       <c r="F76" s="1">
-        <v>25867</v>
+        <v>38259</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -18446,19 +18959,19 @@
         <v>18</v>
       </c>
       <c r="B77" s="1">
-        <v>64</v>
+        <v>128</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D77" s="1">
-        <v>50733</v>
+        <v>87376</v>
       </c>
       <c r="E77" s="1">
-        <v>34.3896484375</v>
+        <v>55.583984375</v>
       </c>
       <c r="F77" s="1">
-        <v>35276</v>
+        <v>59899</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
@@ -18466,19 +18979,19 @@
         <v>18</v>
       </c>
       <c r="B78" s="1">
-        <v>1</v>
+        <v>256</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D78" s="1">
-        <v>38142</v>
+        <v>157235</v>
       </c>
       <c r="E78" s="1">
-        <v>43.9130859375</v>
+        <v>114.1259765625</v>
       </c>
       <c r="F78" s="1">
-        <v>44607</v>
+        <v>103303</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -18486,19 +18999,19 @@
         <v>18</v>
       </c>
       <c r="B79" s="1">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D79" s="1">
-        <v>40983</v>
+        <v>205355</v>
       </c>
       <c r="E79" s="1">
-        <v>60.052734375</v>
+        <v>15.8818359375</v>
       </c>
       <c r="F79" s="1">
-        <v>61650</v>
+        <v>16218</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -18506,19 +19019,19 @@
         <v>18</v>
       </c>
       <c r="B80" s="1">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D80" s="1">
-        <v>219003</v>
+        <v>18449</v>
       </c>
       <c r="E80" s="1">
-        <v>267.9677734375</v>
+        <v>17.857421875</v>
       </c>
       <c r="F80" s="1">
-        <v>327855</v>
+        <v>18299</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -18526,19 +19039,19 @@
         <v>18</v>
       </c>
       <c r="B81" s="1">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D81" s="1">
-        <v>234922</v>
+        <v>207347</v>
       </c>
       <c r="E81" s="1">
-        <v>304.619140625</v>
+        <v>20.181640625</v>
       </c>
       <c r="F81" s="1">
-        <v>312137</v>
+        <v>20638</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
@@ -18546,19 +19059,19 @@
         <v>18</v>
       </c>
       <c r="B82" s="1">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D82" s="1">
-        <v>251670</v>
+        <v>33487</v>
       </c>
       <c r="E82" s="1">
-        <v>381.3505859375</v>
+        <v>25.259765625</v>
       </c>
       <c r="F82" s="1">
-        <v>391003</v>
+        <v>25867</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -18566,19 +19079,19 @@
         <v>18</v>
       </c>
       <c r="B83" s="1">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D83" s="1">
-        <v>285258</v>
+        <v>50733</v>
       </c>
       <c r="E83" s="1">
-        <v>559.9638671875</v>
+        <v>34.3896484375</v>
       </c>
       <c r="F83" s="1">
-        <v>546979</v>
+        <v>35276</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -18586,19 +19099,19 @@
         <v>18</v>
       </c>
       <c r="B84" s="1">
-        <v>256</v>
+        <v>1</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D84" s="1">
-        <v>352182</v>
+        <v>38142</v>
       </c>
       <c r="E84" s="1">
-        <v>842.126953125</v>
+        <v>43.9130859375</v>
       </c>
       <c r="F84" s="1">
-        <v>898484</v>
+        <v>44607</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -18606,19 +19119,19 @@
         <v>18</v>
       </c>
       <c r="B85" s="1">
-        <v>512</v>
+        <v>8</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D85" s="1">
-        <v>922155</v>
+        <v>40983</v>
       </c>
       <c r="E85" s="1">
-        <v>2252.7060546875</v>
+        <v>60.052734375</v>
       </c>
       <c r="F85" s="1">
-        <v>2308339</v>
+        <v>61650</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -18626,19 +19139,19 @@
         <v>18</v>
       </c>
       <c r="B86" s="1">
-        <v>1024</v>
+        <v>16</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D86" s="1">
-        <v>1350176</v>
+        <v>219003</v>
       </c>
       <c r="E86" s="1">
-        <v>3960.66015625</v>
+        <v>267.9677734375</v>
       </c>
       <c r="F86" s="1">
-        <v>4058669</v>
+        <v>327855</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -18646,19 +19159,19 @@
         <v>18</v>
       </c>
       <c r="B87" s="1">
-        <v>1280</v>
+        <v>32</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D87" s="1">
-        <v>1772780</v>
+        <v>234922</v>
       </c>
       <c r="E87" s="1">
-        <v>4994.587890625</v>
+        <v>304.619140625</v>
       </c>
       <c r="F87" s="1">
-        <v>5117864</v>
+        <v>312137</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -18666,19 +19179,19 @@
         <v>18</v>
       </c>
       <c r="B88" s="1">
-        <v>1536</v>
+        <v>64</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D88" s="1">
-        <v>2791972</v>
+        <v>251670</v>
       </c>
       <c r="E88" s="1">
-        <v>5722.361328125</v>
+        <v>381.3505859375</v>
       </c>
       <c r="F88" s="1">
-        <v>5863874</v>
+        <v>391003</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -18686,19 +19199,19 @@
         <v>18</v>
       </c>
       <c r="B89" s="1">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="D89" s="1">
-        <v>71899</v>
+        <v>285258</v>
       </c>
       <c r="E89" s="1">
-        <v>11.1865234375</v>
+        <v>559.9638671875</v>
       </c>
       <c r="F89" s="1">
-        <v>11549</v>
+        <v>546979</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
@@ -18706,19 +19219,19 @@
         <v>18</v>
       </c>
       <c r="B90" s="1">
-        <v>8</v>
+        <v>256</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="D90" s="1">
-        <v>13345</v>
+        <v>352182</v>
       </c>
       <c r="E90" s="1">
-        <v>19.2880859375</v>
+        <v>842.126953125</v>
       </c>
       <c r="F90" s="1">
-        <v>20037</v>
+        <v>898484</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -18726,19 +19239,19 @@
         <v>18</v>
       </c>
       <c r="B91" s="1">
-        <v>16</v>
+        <v>512</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="D91" s="1">
-        <v>25083</v>
+        <v>922155</v>
       </c>
       <c r="E91" s="1">
-        <v>28.5595703125</v>
+        <v>2252.7060546875</v>
       </c>
       <c r="F91" s="1">
-        <v>29740</v>
+        <v>2308339</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
@@ -18746,19 +19259,19 @@
         <v>18</v>
       </c>
       <c r="B92" s="1">
-        <v>32</v>
+        <v>1024</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="D92" s="1">
-        <v>60350</v>
+        <v>1350176</v>
       </c>
       <c r="E92" s="1">
-        <v>47.0234375</v>
+        <v>3960.66015625</v>
       </c>
       <c r="F92" s="1">
-        <v>49071</v>
+        <v>4058669</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
@@ -18766,19 +19279,19 @@
         <v>18</v>
       </c>
       <c r="B93" s="1">
-        <v>64</v>
+        <v>1280</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="D93" s="1">
-        <v>67776</v>
+        <v>1772780</v>
       </c>
       <c r="E93" s="1">
-        <v>83.724609375</v>
+        <v>4994.587890625</v>
       </c>
       <c r="F93" s="1">
-        <v>87499</v>
+        <v>5117864</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -18786,19 +19299,19 @@
         <v>18</v>
       </c>
       <c r="B94" s="1">
-        <v>128</v>
+        <v>1536</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="D94" s="1">
-        <v>124362</v>
+        <v>2791972</v>
       </c>
       <c r="E94" s="1">
-        <v>156.685546875</v>
+        <v>5722.361328125</v>
       </c>
       <c r="F94" s="1">
-        <v>163900</v>
+        <v>5863874</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -18806,19 +19319,19 @@
         <v>18</v>
       </c>
       <c r="B95" s="1">
-        <v>256</v>
+        <v>1</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D95" s="1">
-        <v>236992</v>
+        <v>285821</v>
       </c>
       <c r="E95" s="1">
-        <v>303.8046875</v>
+        <v>18.6181640625</v>
       </c>
       <c r="F95" s="1">
-        <v>317923</v>
+        <v>19129</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -18826,19 +19339,19 @@
         <v>18</v>
       </c>
       <c r="B96" s="1">
-        <v>512</v>
+        <v>8</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D96" s="1">
-        <v>463360</v>
+        <v>20962</v>
       </c>
       <c r="E96" s="1">
-        <v>599.650390625</v>
+        <v>26.7197265625</v>
       </c>
       <c r="F96" s="1">
-        <v>627606</v>
+        <v>27640</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
@@ -18846,19 +19359,259 @@
         <v>18</v>
       </c>
       <c r="B97" s="1">
-        <v>1024</v>
+        <v>16</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D97" s="1">
-        <v>927239</v>
+        <v>32742</v>
       </c>
       <c r="E97" s="1">
-        <v>1197.705078125</v>
+        <v>35.982421875</v>
       </c>
       <c r="F97" s="1">
-        <v>1256716</v>
+        <v>37340</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>18</v>
+      </c>
+      <c r="B98" s="1">
+        <v>32</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D98" s="1">
+        <v>47098</v>
+      </c>
+      <c r="E98" s="1">
+        <v>54.0966796875</v>
+      </c>
+      <c r="F98" s="1">
+        <v>129733</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>18</v>
+      </c>
+      <c r="B99" s="1">
+        <v>64</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D99" s="1">
+        <v>185845</v>
+      </c>
+      <c r="E99" s="1">
+        <v>91.232421875</v>
+      </c>
+      <c r="F99" s="1">
+        <v>95187</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>18</v>
+      </c>
+      <c r="B100" s="1">
+        <v>128</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D100" s="1">
+        <v>132575</v>
+      </c>
+      <c r="E100" s="1">
+        <v>164.294921875</v>
+      </c>
+      <c r="F100" s="1">
+        <v>171690</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>18</v>
+      </c>
+      <c r="B101" s="1">
+        <v>256</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D101" s="1">
+        <v>245851</v>
+      </c>
+      <c r="E101" s="1">
+        <v>311.4609375</v>
+      </c>
+      <c r="F101" s="1">
+        <v>325763</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>18</v>
+      </c>
+      <c r="B102" s="1">
+        <v>512</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D102" s="1">
+        <v>473347</v>
+      </c>
+      <c r="E102" s="1">
+        <v>607.216796875</v>
+      </c>
+      <c r="F102" s="1">
+        <v>635353</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>18</v>
+      </c>
+      <c r="B103" s="1">
+        <v>1024</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D103" s="1">
+        <v>1370147</v>
+      </c>
+      <c r="E103" s="1">
+        <v>1287.9794921875</v>
+      </c>
+      <c r="F103" s="1">
+        <v>1307497</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>18</v>
+      </c>
+      <c r="B104" s="1">
+        <v>1280</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D104" s="1">
+        <v>1800223</v>
+      </c>
+      <c r="E104" s="1">
+        <v>1665.271484375</v>
+      </c>
+      <c r="F104" s="1">
+        <v>1596094</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>18</v>
+      </c>
+      <c r="B105" s="1">
+        <v>1536</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D105" s="1">
+        <v>2178449</v>
+      </c>
+      <c r="E105" s="1">
+        <v>1789.921875</v>
+      </c>
+      <c r="F105" s="1">
+        <v>1920954</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>18</v>
+      </c>
+      <c r="B106" s="1">
+        <v>2048</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D106" s="1">
+        <v>2735426</v>
+      </c>
+      <c r="E106" s="1">
+        <v>2430.4619140625</v>
+      </c>
+      <c r="F106" s="1">
+        <v>2541582</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>18</v>
+      </c>
+      <c r="B107" s="1">
+        <v>2304</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D107" s="1">
+        <v>3458016</v>
+      </c>
+      <c r="E107" s="1">
+        <v>2746.7294921875</v>
+      </c>
+      <c r="F107" s="1">
+        <v>2858895</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>18</v>
+      </c>
+      <c r="B108" s="1">
+        <v>2560</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D108" s="1">
+        <v>3878785</v>
+      </c>
+      <c r="E108" s="1">
+        <v>3005.7177734375</v>
+      </c>
+      <c r="F108" s="1">
+        <v>3178637</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>18</v>
+      </c>
+      <c r="B109" s="1">
+        <v>3072</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D109" s="1">
+        <v>4360095</v>
+      </c>
+      <c r="E109" s="1">
+        <v>3606.0419921875</v>
+      </c>
+      <c r="F109" s="1">
+        <v>3800009</v>
       </c>
     </row>
   </sheetData>

</xml_diff>